<commit_message>
red_x not forced to be non-negative
</commit_message>
<xml_diff>
--- a/Error_vs_Frame_vs_ExpPara.xlsx
+++ b/Error_vs_Frame_vs_ExpPara.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="96" windowWidth="22116" windowHeight="10872" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="96" windowWidth="22116" windowHeight="9540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>lambda [m]</t>
   </si>
@@ -224,14 +224,30 @@
   <si>
     <t>N_fac</t>
   </si>
+  <si>
+    <t>EQ 12</t>
+  </si>
+  <si>
+    <t>EQ 7</t>
+  </si>
+  <si>
+    <t>δ(x)</t>
+  </si>
+  <si>
+    <t>y1</t>
+  </si>
+  <si>
+    <t>y2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0E+00"/>
-    <numFmt numFmtId="173" formatCode="0.0%"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="0E+00"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -317,10 +333,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -329,13 +345,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
@@ -415,7 +432,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'min rel. error of D'!$B$6:$B$56</c:f>
+              <c:f>'min rel. error of D'!$B$7:$B$57</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="51"/>
@@ -577,162 +594,162 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'min rel. error of D'!$C$6:$C$56</c:f>
+              <c:f>'min rel. error of D'!$C$7:$C$57</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>0.84596965038972016</c:v>
+                  <c:v>0.76655347622849213</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.76520834028295548</c:v>
+                  <c:v>0.69337370792523434</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.69330389216948318</c:v>
+                  <c:v>0.6282193556003236</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.62899738110065562</c:v>
+                  <c:v>0.5699496770353456</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.57127664461541194</c:v>
+                  <c:v>0.51764752744540565</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.51931369987987008</c:v>
+                  <c:v>0.47056265164194316</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.47242087317234938</c:v>
+                  <c:v>0.42807193190244563</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.43001937991202943</c:v>
+                  <c:v>0.38965091757763648</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.39161638666470672</c:v>
+                  <c:v>0.35485304042240623</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.35678797224401232</c:v>
+                  <c:v>0.32329417523922777</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.32516626721236158</c:v>
+                  <c:v>0.2946409866702086</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.29642960166227339</c:v>
+                  <c:v>0.26860200186444427</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.27029485097069045</c:v>
+                  <c:v>0.24492067478164786</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.24651140926367104</c:v>
+                  <c:v>0.22336992540335199</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.22485638344942224</c:v>
+                  <c:v>0.20374778493048396</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.20513071336383795</c:v>
+                  <c:v>0.18587388015378753</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.18715600257032558</c:v>
+                  <c:v>0.1695865617652127</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.17077190046800397</c:v>
+                  <c:v>0.15474053222309928</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.15583391668987037</c:v>
+                  <c:v>0.1412048653257135</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.14221157806256524</c:v>
+                  <c:v>0.12886133618809978</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.12978685987591285</c:v>
+                  <c:v>0.1176029997776267</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.11845283909444546</c:v>
+                  <c:v>0.1073329705565106</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.1081125289846248</c:v>
+                  <c:v>9.7963366509471655E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9.867786352493739E-2</c:v>
+                  <c:v>8.9414388893259825E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>9.0068806692533518E-2</c:v>
+                  <c:v>8.1613515139824705E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8.2212566842306808E-2</c:v>
+                  <c:v>7.4494786986277151E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.504290032111624E-2</c:v>
+                  <c:v>6.7998179462962563E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6.8499491490535816E-2</c:v>
+                  <c:v>6.2069039117141726E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6.2527398686673424E-2</c:v>
+                  <c:v>5.665758198383803E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5.7076557488790258E-2</c:v>
+                  <c:v>5.1718443485569289E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>5.2101334121618013E-2</c:v>
+                  <c:v>4.721027375943055E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4.7560122970763084E-2</c:v>
+                  <c:v>4.3095372956107665E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.3414983115160774E-2</c:v>
+                  <c:v>3.9339361893179554E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.9631309527157842E-2</c:v>
+                  <c:v>3.5910884121593496E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.6177535198892025E-2</c:v>
+                  <c:v>3.2781336015203111E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.3024860953244389E-2</c:v>
+                  <c:v>2.9924621945964437E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.0147010111744775E-2</c:v>
+                  <c:v>2.7316931982616047E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.7520005538061682E-2</c:v>
+                  <c:v>2.4936539864415071E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2.5121966867719864E-2</c:v>
+                  <c:v>2.2763619266100415E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2.2932925983009386E-2</c:v>
+                  <c:v>2.0780076595263364E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2.0934659004892085E-2</c:v>
+                  <c:v>1.8969398756167408E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1.9110533257504034E-2</c:v>
+                  <c:v>1.7316514480597893E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1.7445367820655866E-2</c:v>
+                  <c:v>1.5807667971123859E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1.5925306425555768E-2</c:v>
+                  <c:v>1.443030372885119E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.4537701572018696E-2</c:v>
+                  <c:v>1.3172961549234748E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.3271008854247743E-2</c:v>
+                  <c:v>1.2025180768123598E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1.2114690578957109E-2</c:v>
+                  <c:v>1.0977412927820776E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.1059127845846051E-2</c:v>
+                  <c:v>1.0020942111083115E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.0095540337623584E-2</c:v>
+                  <c:v>9.1478122609306815E-3</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>9.2159131360812739E-3</c:v>
+                  <c:v>8.3507608669276309E-3</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>8.4129299430834789E-3</c:v>
+                  <c:v>7.6231584551130329E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -747,11 +764,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="148014784"/>
-        <c:axId val="148013632"/>
+        <c:axId val="243197632"/>
+        <c:axId val="243198208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="148014784"/>
+        <c:axId val="243197632"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -788,12 +805,12 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="148013632"/>
+        <c:crossAx val="243198208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="148013632"/>
+        <c:axId val="243198208"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -828,7 +845,7 @@
         <c:spPr>
           <a:ln w="9525"/>
         </c:spPr>
-        <c:crossAx val="148014784"/>
+        <c:crossAx val="243197632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -854,16 +871,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>179070</xdr:rowOff>
+      <xdr:rowOff>125730</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>769620</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1175,7 +1192,7 @@
   <dimension ref="B1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1191,7 +1208,7 @@
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1205,7 +1222,7 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="7"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1213,11 +1230,11 @@
         <v>1</v>
       </c>
       <c r="E3" s="5">
-        <v>0.1</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="B4" s="7"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
@@ -1226,14 +1243,14 @@
       </c>
       <c r="E4" s="1">
         <f>0.21*E2/E3</f>
-        <v>1.1172000000000001E-6</v>
+        <v>8.9376000000000006E-8</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="7"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
@@ -1242,11 +1259,11 @@
       </c>
       <c r="E5" s="1">
         <f>2.35*E4</f>
-        <v>2.6254200000000004E-6</v>
+        <v>2.1003360000000002E-7</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1256,11 +1273,11 @@
         <v>16</v>
       </c>
       <c r="E7" s="1">
-        <v>8.0000000000000002E-8</v>
+        <v>5.9999999999999995E-8</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="7"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="3" t="s">
         <v>2</v>
       </c>
@@ -1272,7 +1289,7 @@
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="7"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="3" t="s">
         <v>2</v>
       </c>
@@ -1284,7 +1301,7 @@
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="7"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="4" t="s">
         <v>3</v>
       </c>
@@ -1296,7 +1313,7 @@
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="7"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="4" t="s">
         <v>3</v>
       </c>
@@ -1305,14 +1322,14 @@
       </c>
       <c r="E11" s="1">
         <f>E10*E9/(6*PI()*E8*(E7/2))</f>
-        <v>5.3650574273977089E-12</v>
+        <v>7.1534099031969463E-12</v>
       </c>
       <c r="F11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="12" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -1329,7 +1346,7 @@
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="7"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="3" t="s">
         <v>2</v>
       </c>
@@ -1337,47 +1354,47 @@
         <v>13</v>
       </c>
       <c r="E15" s="5">
-        <v>700</v>
+        <v>2480</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="7"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>19</v>
       </c>
       <c r="E16" s="2">
         <f>1/E15</f>
-        <v>1.4285714285714286E-3</v>
+        <v>4.032258064516129E-4</v>
       </c>
       <c r="F16" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="7"/>
+      <c r="B17" s="12"/>
       <c r="C17" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E17" s="5">
         <f>1/6*E14/E16</f>
-        <v>2.3333333333333334E-2</v>
+        <v>8.2666666666666666E-2</v>
       </c>
       <c r="F17" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="7"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>22</v>
       </c>
       <c r="E18" s="5">
@@ -1388,67 +1405,67 @@
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D19" s="8"/>
+      <c r="D19" s="7"/>
     </row>
     <row r="20" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="12" t="s">
         <v>32</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E20" s="1">
         <f>E4/SQRT(E18)</f>
-        <v>3.5328966019401138E-8</v>
+        <v>2.8263172815520908E-9</v>
       </c>
       <c r="F20" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="7"/>
+      <c r="B21" s="12"/>
       <c r="C21" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E21" s="1">
         <f>E20*SQRT(1+E11*E14/(E4^2))</f>
-        <v>3.534414875881834E-8</v>
+        <v>3.0689984289079374E-9</v>
       </c>
       <c r="F21" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="7"/>
+      <c r="B22" s="12"/>
       <c r="C22" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="7" t="s">
         <v>29</v>
       </c>
       <c r="E22" s="1">
         <f>E20^2/(E11*E16)*(1+E11*E14/(E4^2))-1/3*E14/E16</f>
-        <v>0.11632249195338956</v>
+        <v>-0.16206796707017168</v>
       </c>
       <c r="F22" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="7"/>
-      <c r="E23" s="9" t="str">
+      <c r="B23" s="12"/>
+      <c r="E23" s="8" t="str">
         <f>IF(E22&lt;(2/3)," quasi optimal fit possible", "not optimal fit possible")</f>
         <v xml:space="preserve"> quasi optimal fit possible</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="B24" s="7"/>
+      <c r="B24" s="12"/>
       <c r="C24" s="4" t="s">
         <v>3</v>
       </c>
@@ -1457,14 +1474,14 @@
       </c>
       <c r="E24" s="1">
         <f>1+E4^2/(E11*E16)</f>
-        <v>163.84915862005619</v>
+        <v>3.7693662631616411</v>
       </c>
       <c r="F24" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="7"/>
+      <c r="B25" s="12"/>
       <c r="C25" s="4" t="s">
         <v>3</v>
       </c>
@@ -1486,565 +1503,804 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C61"/>
+  <dimension ref="B2:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.5546875" style="10"/>
+    <col min="3" max="3" width="11.5546875" style="9"/>
+    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="6">
         <f>Inputs!E22</f>
-        <v>0.11632249195338956</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+        <v>-0.16206796707017168</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="11">
+        <f>1/SQRT(1+2*$C$2)</f>
+        <v>1.216382943469255</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>38</v>
       </c>
       <c r="C3" s="6">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="11">
+        <f>(1+$C$2)/((1+2*$C$2)^(3/2))</f>
+        <v>1.5080639497321757</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="11">
+        <f>(1-F2)/SQRT(F3-(F2)^2)</f>
+        <v>-1.282271049205649</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="11">
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="10">
         <v>10</v>
       </c>
-      <c r="C6" s="10">
-        <f>SQRT(2/(B6-1)*(1+2*SQRT(1+2*$C$2)))</f>
-        <v>0.84596965038972016</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="11">
-        <f>$C$3*B6</f>
+      <c r="C7" s="9">
+        <f>SQRT(2/(B7-1)*(1+2*SQRT(1+2*$C$2)))</f>
+        <v>0.76655347622849213</v>
+      </c>
+      <c r="D7" s="9">
+        <f>SQRT(2/(B7-1)*(1+$F$4^2))</f>
+        <v>0.76655347622849523</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="10">
+        <f>$C$3*B7</f>
         <v>12</v>
       </c>
-      <c r="C7" s="10">
-        <f t="shared" ref="C7:C56" si="0">SQRT(2/(B7-1)*(1+2*SQRT(1+2*$C$2)))</f>
-        <v>0.76520834028295548</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="11">
-        <f t="shared" ref="B8:B61" si="1">$C$3*B7</f>
+      <c r="C8" s="9">
+        <f t="shared" ref="C8:C57" si="0">SQRT(2/(B8-1)*(1+2*SQRT(1+2*$C$2)))</f>
+        <v>0.69337370792523434</v>
+      </c>
+      <c r="D8" s="9">
+        <f t="shared" ref="D8:D57" si="1">SQRT(2/(B8-1)*(1+$F$4^2))</f>
+        <v>0.69337370792523711</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="10">
+        <f t="shared" ref="B9:B57" si="2">$C$3*B8</f>
         <v>14.399999999999999</v>
       </c>
-      <c r="C8" s="10">
-        <f t="shared" si="0"/>
-        <v>0.69330389216948318</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="11">
-        <f t="shared" si="1"/>
+      <c r="C9" s="9">
+        <f t="shared" si="0"/>
+        <v>0.6282193556003236</v>
+      </c>
+      <c r="D9" s="9">
+        <f t="shared" si="1"/>
+        <v>0.62821935560032616</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="10">
+        <f t="shared" si="2"/>
         <v>17.279999999999998</v>
       </c>
-      <c r="C9" s="10">
-        <f t="shared" si="0"/>
-        <v>0.62899738110065562</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="11">
-        <f t="shared" si="1"/>
+      <c r="C10" s="9">
+        <f t="shared" si="0"/>
+        <v>0.5699496770353456</v>
+      </c>
+      <c r="D10" s="9">
+        <f t="shared" si="1"/>
+        <v>0.56994967703534793</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="10">
+        <f t="shared" si="2"/>
         <v>20.735999999999997</v>
       </c>
-      <c r="C10" s="10">
-        <f t="shared" si="0"/>
-        <v>0.57127664461541194</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="11">
-        <f t="shared" si="1"/>
+      <c r="C11" s="9">
+        <f t="shared" si="0"/>
+        <v>0.51764752744540565</v>
+      </c>
+      <c r="D11" s="9">
+        <f t="shared" si="1"/>
+        <v>0.51764752744540776</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B12" s="10">
+        <f t="shared" si="2"/>
         <v>24.883199999999995</v>
       </c>
-      <c r="C11" s="10">
-        <f t="shared" si="0"/>
-        <v>0.51931369987987008</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B12" s="11">
-        <f t="shared" si="1"/>
+      <c r="C12" s="9">
+        <f t="shared" si="0"/>
+        <v>0.47056265164194316</v>
+      </c>
+      <c r="D12" s="9">
+        <f t="shared" si="1"/>
+        <v>0.47056265164194505</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B13" s="10">
+        <f t="shared" si="2"/>
         <v>29.859839999999991</v>
       </c>
-      <c r="C12" s="10">
-        <f t="shared" si="0"/>
-        <v>0.47242087317234938</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="11">
-        <f t="shared" si="1"/>
+      <c r="C13" s="9">
+        <f t="shared" si="0"/>
+        <v>0.42807193190244563</v>
+      </c>
+      <c r="D13" s="9">
+        <f t="shared" si="1"/>
+        <v>0.42807193190244736</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="10">
+        <f t="shared" si="2"/>
         <v>35.831807999999988</v>
       </c>
-      <c r="C13" s="10">
-        <f t="shared" si="0"/>
-        <v>0.43001937991202943</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B14" s="11">
-        <f t="shared" si="1"/>
+      <c r="C14" s="9">
+        <f t="shared" si="0"/>
+        <v>0.38965091757763648</v>
+      </c>
+      <c r="D14" s="9">
+        <f t="shared" si="1"/>
+        <v>0.38965091757763809</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="10">
+        <f t="shared" si="2"/>
         <v>42.998169599999983</v>
       </c>
-      <c r="C14" s="10">
-        <f t="shared" si="0"/>
-        <v>0.39161638666470672</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B15" s="11">
-        <f t="shared" si="1"/>
+      <c r="C15" s="9">
+        <f t="shared" si="0"/>
+        <v>0.35485304042240623</v>
+      </c>
+      <c r="D15" s="9">
+        <f t="shared" si="1"/>
+        <v>0.35485304042240767</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B16" s="10">
+        <f t="shared" si="2"/>
         <v>51.597803519999978</v>
       </c>
-      <c r="C15" s="10">
-        <f t="shared" si="0"/>
-        <v>0.35678797224401232</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B16" s="11">
-        <f t="shared" si="1"/>
+      <c r="C16" s="9">
+        <f t="shared" si="0"/>
+        <v>0.32329417523922777</v>
+      </c>
+      <c r="D16" s="9">
+        <f t="shared" si="1"/>
+        <v>0.32329417523922904</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="10">
+        <f t="shared" si="2"/>
         <v>61.917364223999968</v>
       </c>
-      <c r="C16" s="10">
-        <f t="shared" si="0"/>
-        <v>0.32516626721236158</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="11">
-        <f t="shared" si="1"/>
+      <c r="C17" s="9">
+        <f t="shared" si="0"/>
+        <v>0.2946409866702086</v>
+      </c>
+      <c r="D17" s="9">
+        <f t="shared" si="1"/>
+        <v>0.29464098667020977</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="10">
+        <f t="shared" si="2"/>
         <v>74.300837068799964</v>
       </c>
-      <c r="C17" s="10">
-        <f t="shared" si="0"/>
-        <v>0.29642960166227339</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="11">
-        <f t="shared" si="1"/>
+      <c r="C18" s="9">
+        <f t="shared" si="0"/>
+        <v>0.26860200186444427</v>
+      </c>
+      <c r="D18" s="9">
+        <f t="shared" si="1"/>
+        <v>0.26860200186444538</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="10">
+        <f t="shared" si="2"/>
         <v>89.16100448255996</v>
       </c>
-      <c r="C18" s="10">
-        <f t="shared" si="0"/>
-        <v>0.27029485097069045</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" s="11">
-        <f t="shared" si="1"/>
+      <c r="C19" s="9">
+        <f t="shared" si="0"/>
+        <v>0.24492067478164786</v>
+      </c>
+      <c r="D19" s="9">
+        <f t="shared" si="1"/>
+        <v>0.24492067478164886</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="10">
+        <f t="shared" si="2"/>
         <v>106.99320537907195</v>
       </c>
-      <c r="C19" s="10">
-        <f t="shared" si="0"/>
-        <v>0.24651140926367104</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B20" s="11">
-        <f t="shared" si="1"/>
+      <c r="C20" s="9">
+        <f t="shared" si="0"/>
+        <v>0.22336992540335199</v>
+      </c>
+      <c r="D20" s="9">
+        <f t="shared" si="1"/>
+        <v>0.22336992540335288</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="10">
+        <f t="shared" si="2"/>
         <v>128.39184645488635</v>
       </c>
-      <c r="C20" s="10">
-        <f t="shared" si="0"/>
-        <v>0.22485638344942224</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21" s="11">
-        <f t="shared" si="1"/>
+      <c r="C21" s="9">
+        <f t="shared" si="0"/>
+        <v>0.20374778493048396</v>
+      </c>
+      <c r="D21" s="9">
+        <f t="shared" si="1"/>
+        <v>0.20374778493048479</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="10">
+        <f t="shared" si="2"/>
         <v>154.07021574586361</v>
       </c>
-      <c r="C21" s="10">
-        <f t="shared" si="0"/>
-        <v>0.20513071336383795</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B22" s="11">
-        <f t="shared" si="1"/>
+      <c r="C22" s="9">
+        <f t="shared" si="0"/>
+        <v>0.18587388015378753</v>
+      </c>
+      <c r="D22" s="9">
+        <f t="shared" si="1"/>
+        <v>0.18587388015378828</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="10">
+        <f t="shared" si="2"/>
         <v>184.88425889503631</v>
       </c>
-      <c r="C22" s="10">
-        <f t="shared" si="0"/>
-        <v>0.18715600257032558</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B23" s="11">
-        <f t="shared" si="1"/>
+      <c r="C23" s="9">
+        <f t="shared" si="0"/>
+        <v>0.1695865617652127</v>
+      </c>
+      <c r="D23" s="9">
+        <f t="shared" si="1"/>
+        <v>0.16958656176521339</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" s="10">
+        <f t="shared" si="2"/>
         <v>221.86111067404357</v>
       </c>
-      <c r="C23" s="10">
-        <f t="shared" si="0"/>
-        <v>0.17077190046800397</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B24" s="11">
-        <f t="shared" si="1"/>
+      <c r="C24" s="9">
+        <f t="shared" si="0"/>
+        <v>0.15474053222309928</v>
+      </c>
+      <c r="D24" s="9">
+        <f t="shared" si="1"/>
+        <v>0.15474053222309991</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" s="10">
+        <f t="shared" si="2"/>
         <v>266.23333280885225</v>
       </c>
-      <c r="C24" s="10">
-        <f t="shared" si="0"/>
-        <v>0.15583391668987037</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B25" s="11">
-        <f t="shared" si="1"/>
+      <c r="C25" s="9">
+        <f t="shared" si="0"/>
+        <v>0.1412048653257135</v>
+      </c>
+      <c r="D25" s="9">
+        <f t="shared" si="1"/>
+        <v>0.14120486532571408</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B26" s="10">
+        <f t="shared" si="2"/>
         <v>319.47999937062269</v>
       </c>
-      <c r="C25" s="10">
-        <f t="shared" si="0"/>
-        <v>0.14221157806256524</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B26" s="11">
-        <f t="shared" si="1"/>
+      <c r="C26" s="9">
+        <f t="shared" si="0"/>
+        <v>0.12886133618809978</v>
+      </c>
+      <c r="D26" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12886133618810028</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B27" s="10">
+        <f t="shared" si="2"/>
         <v>383.37599924474722</v>
       </c>
-      <c r="C26" s="10">
-        <f t="shared" si="0"/>
-        <v>0.12978685987591285</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B27" s="11">
-        <f t="shared" si="1"/>
+      <c r="C27" s="9">
+        <f t="shared" si="0"/>
+        <v>0.1176029997776267</v>
+      </c>
+      <c r="D27" s="9">
+        <f t="shared" si="1"/>
+        <v>0.11760299977762717</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B28" s="10">
+        <f t="shared" si="2"/>
         <v>460.05119909369665</v>
       </c>
-      <c r="C27" s="10">
-        <f t="shared" si="0"/>
-        <v>0.11845283909444546</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B28" s="11">
-        <f t="shared" si="1"/>
+      <c r="C28" s="9">
+        <f t="shared" si="0"/>
+        <v>0.1073329705565106</v>
+      </c>
+      <c r="D28" s="9">
+        <f t="shared" si="1"/>
+        <v>0.10733297055651105</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B29" s="10">
+        <f t="shared" si="2"/>
         <v>552.06143891243596</v>
       </c>
-      <c r="C28" s="10">
-        <f t="shared" si="0"/>
-        <v>0.1081125289846248</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B29" s="11">
-        <f t="shared" si="1"/>
+      <c r="C29" s="9">
+        <f t="shared" si="0"/>
+        <v>9.7963366509471655E-2</v>
+      </c>
+      <c r="D29" s="9">
+        <f t="shared" si="1"/>
+        <v>9.7963366509472044E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B30" s="10">
+        <f t="shared" si="2"/>
         <v>662.47372669492313</v>
       </c>
-      <c r="C29" s="10">
-        <f t="shared" si="0"/>
-        <v>9.867786352493739E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B30" s="11">
-        <f t="shared" si="1"/>
+      <c r="C30" s="9">
+        <f t="shared" si="0"/>
+        <v>8.9414388893259825E-2</v>
+      </c>
+      <c r="D30" s="9">
+        <f t="shared" si="1"/>
+        <v>8.9414388893260172E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B31" s="10">
+        <f t="shared" si="2"/>
         <v>794.96847203390769</v>
       </c>
-      <c r="C30" s="10">
-        <f t="shared" si="0"/>
-        <v>9.0068806692533518E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B31" s="11">
-        <f t="shared" si="1"/>
+      <c r="C31" s="9">
+        <f t="shared" si="0"/>
+        <v>8.1613515139824705E-2</v>
+      </c>
+      <c r="D31" s="9">
+        <f t="shared" si="1"/>
+        <v>8.1613515139825038E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B32" s="10">
+        <f t="shared" si="2"/>
         <v>953.9621664406892</v>
       </c>
-      <c r="C31" s="10">
-        <f t="shared" si="0"/>
-        <v>8.2212566842306808E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B32" s="11">
-        <f t="shared" si="1"/>
+      <c r="C32" s="9">
+        <f t="shared" si="0"/>
+        <v>7.4494786986277151E-2</v>
+      </c>
+      <c r="D32" s="9">
+        <f t="shared" si="1"/>
+        <v>7.4494786986277456E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B33" s="10">
+        <f t="shared" si="2"/>
         <v>1144.7545997288271</v>
       </c>
-      <c r="C32" s="10">
-        <f t="shared" si="0"/>
-        <v>7.504290032111624E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B33" s="11">
-        <f t="shared" si="1"/>
+      <c r="C33" s="9">
+        <f t="shared" si="0"/>
+        <v>6.7998179462962563E-2</v>
+      </c>
+      <c r="D33" s="9">
+        <f t="shared" si="1"/>
+        <v>6.7998179462962827E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B34" s="10">
+        <f t="shared" si="2"/>
         <v>1373.7055196745926</v>
       </c>
-      <c r="C33" s="10">
-        <f t="shared" si="0"/>
-        <v>6.8499491490535816E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B34" s="11">
-        <f t="shared" si="1"/>
+      <c r="C34" s="9">
+        <f t="shared" si="0"/>
+        <v>6.2069039117141726E-2</v>
+      </c>
+      <c r="D34" s="9">
+        <f t="shared" si="1"/>
+        <v>6.2069039117141976E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B35" s="10">
+        <f t="shared" si="2"/>
         <v>1648.4466236095111</v>
       </c>
-      <c r="C34" s="10">
-        <f t="shared" si="0"/>
-        <v>6.2527398686673424E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B35" s="11">
-        <f t="shared" si="1"/>
+      <c r="C35" s="9">
+        <f t="shared" si="0"/>
+        <v>5.665758198383803E-2</v>
+      </c>
+      <c r="D35" s="9">
+        <f t="shared" si="1"/>
+        <v>5.6657581983838259E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B36" s="10">
+        <f t="shared" si="2"/>
         <v>1978.1359483314131</v>
       </c>
-      <c r="C35" s="10">
-        <f t="shared" si="0"/>
-        <v>5.7076557488790258E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B36" s="11">
-        <f t="shared" si="1"/>
+      <c r="C36" s="9">
+        <f t="shared" si="0"/>
+        <v>5.1718443485569289E-2</v>
+      </c>
+      <c r="D36" s="9">
+        <f t="shared" si="1"/>
+        <v>5.171844348556949E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B37" s="10">
+        <f t="shared" si="2"/>
         <v>2373.7631379976956</v>
       </c>
-      <c r="C36" s="10">
-        <f t="shared" si="0"/>
-        <v>5.2101334121618013E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B37" s="11">
-        <f t="shared" si="1"/>
+      <c r="C37" s="9">
+        <f t="shared" si="0"/>
+        <v>4.721027375943055E-2</v>
+      </c>
+      <c r="D37" s="9">
+        <f t="shared" si="1"/>
+        <v>4.7210273759430738E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B38" s="10">
+        <f t="shared" si="2"/>
         <v>2848.5157655972348</v>
       </c>
-      <c r="C37" s="10">
-        <f t="shared" si="0"/>
-        <v>4.7560122970763084E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B38" s="11">
-        <f t="shared" si="1"/>
+      <c r="C38" s="9">
+        <f t="shared" si="0"/>
+        <v>4.3095372956107665E-2</v>
+      </c>
+      <c r="D38" s="9">
+        <f t="shared" si="1"/>
+        <v>4.3095372956107839E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B39" s="10">
+        <f t="shared" si="2"/>
         <v>3418.2189187166819</v>
       </c>
-      <c r="C38" s="10">
-        <f t="shared" si="0"/>
-        <v>4.3414983115160774E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B39" s="11">
-        <f t="shared" si="1"/>
+      <c r="C39" s="9">
+        <f t="shared" si="0"/>
+        <v>3.9339361893179554E-2</v>
+      </c>
+      <c r="D39" s="9">
+        <f t="shared" si="1"/>
+        <v>3.9339361893179714E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B40" s="10">
+        <f t="shared" si="2"/>
         <v>4101.8627024600182</v>
       </c>
-      <c r="C39" s="10">
-        <f t="shared" si="0"/>
-        <v>3.9631309527157842E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B40" s="11">
-        <f t="shared" si="1"/>
+      <c r="C40" s="9">
+        <f t="shared" si="0"/>
+        <v>3.5910884121593496E-2</v>
+      </c>
+      <c r="D40" s="9">
+        <f t="shared" si="1"/>
+        <v>3.5910884121593642E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B41" s="10">
+        <f t="shared" si="2"/>
         <v>4922.2352429520215</v>
       </c>
-      <c r="C40" s="10">
-        <f t="shared" si="0"/>
-        <v>3.6177535198892025E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B41" s="11">
-        <f t="shared" si="1"/>
+      <c r="C41" s="9">
+        <f t="shared" si="0"/>
+        <v>3.2781336015203111E-2</v>
+      </c>
+      <c r="D41" s="9">
+        <f t="shared" si="1"/>
+        <v>3.2781336015203236E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B42" s="10">
+        <f t="shared" si="2"/>
         <v>5906.6822915424254</v>
       </c>
-      <c r="C41" s="10">
-        <f t="shared" si="0"/>
-        <v>3.3024860953244389E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B42" s="11">
-        <f t="shared" si="1"/>
+      <c r="C42" s="9">
+        <f t="shared" si="0"/>
+        <v>2.9924621945964437E-2</v>
+      </c>
+      <c r="D42" s="9">
+        <f t="shared" si="1"/>
+        <v>2.9924621945964555E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B43" s="10">
+        <f t="shared" si="2"/>
         <v>7088.0187498509104</v>
       </c>
-      <c r="C42" s="10">
-        <f t="shared" si="0"/>
-        <v>3.0147010111744775E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="11">
-        <f t="shared" si="1"/>
+      <c r="C43" s="9">
+        <f t="shared" si="0"/>
+        <v>2.7316931982616047E-2</v>
+      </c>
+      <c r="D43" s="9">
+        <f t="shared" si="1"/>
+        <v>2.7316931982616158E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B44" s="10">
+        <f t="shared" si="2"/>
         <v>8505.6224998210928</v>
       </c>
-      <c r="C43" s="10">
-        <f t="shared" si="0"/>
-        <v>2.7520005538061682E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="11">
-        <f t="shared" si="1"/>
+      <c r="C44" s="9">
+        <f t="shared" si="0"/>
+        <v>2.4936539864415071E-2</v>
+      </c>
+      <c r="D44" s="9">
+        <f t="shared" si="1"/>
+        <v>2.4936539864415172E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B45" s="10">
+        <f t="shared" si="2"/>
         <v>10206.746999785311</v>
       </c>
-      <c r="C44" s="10">
-        <f t="shared" si="0"/>
-        <v>2.5121966867719864E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="11">
-        <f t="shared" si="1"/>
+      <c r="C45" s="9">
+        <f t="shared" si="0"/>
+        <v>2.2763619266100415E-2</v>
+      </c>
+      <c r="D45" s="9">
+        <f t="shared" si="1"/>
+        <v>2.2763619266100505E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B46" s="10">
+        <f t="shared" si="2"/>
         <v>12248.096399742373</v>
       </c>
-      <c r="C45" s="10">
-        <f t="shared" si="0"/>
-        <v>2.2932925983009386E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="11">
-        <f t="shared" si="1"/>
+      <c r="C46" s="9">
+        <f t="shared" si="0"/>
+        <v>2.0780076595263364E-2</v>
+      </c>
+      <c r="D46" s="9">
+        <f t="shared" si="1"/>
+        <v>2.0780076595263451E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B47" s="10">
+        <f t="shared" si="2"/>
         <v>14697.715679690848</v>
       </c>
-      <c r="C46" s="10">
-        <f t="shared" si="0"/>
-        <v>2.0934659004892085E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="11">
-        <f t="shared" si="1"/>
+      <c r="C47" s="9">
+        <f t="shared" si="0"/>
+        <v>1.8969398756167408E-2</v>
+      </c>
+      <c r="D47" s="9">
+        <f t="shared" si="1"/>
+        <v>1.8969398756167485E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B48" s="10">
+        <f t="shared" si="2"/>
         <v>17637.258815629015</v>
       </c>
-      <c r="C47" s="10">
-        <f t="shared" si="0"/>
-        <v>1.9110533257504034E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B48" s="11">
-        <f t="shared" si="1"/>
+      <c r="C48" s="9">
+        <f t="shared" si="0"/>
+        <v>1.7316514480597893E-2</v>
+      </c>
+      <c r="D48" s="9">
+        <f t="shared" si="1"/>
+        <v>1.7316514480597966E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B49" s="10">
+        <f t="shared" si="2"/>
         <v>21164.710578754817</v>
       </c>
-      <c r="C48" s="10">
-        <f t="shared" si="0"/>
-        <v>1.7445367820655866E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B49" s="11">
-        <f t="shared" si="1"/>
+      <c r="C49" s="9">
+        <f t="shared" si="0"/>
+        <v>1.5807667971123859E-2</v>
+      </c>
+      <c r="D49" s="9">
+        <f t="shared" si="1"/>
+        <v>1.5807667971123922E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B50" s="10">
+        <f t="shared" si="2"/>
         <v>25397.652694505781</v>
       </c>
-      <c r="C49" s="10">
-        <f t="shared" si="0"/>
-        <v>1.5925306425555768E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B50" s="11">
-        <f t="shared" si="1"/>
+      <c r="C50" s="9">
+        <f t="shared" si="0"/>
+        <v>1.443030372885119E-2</v>
+      </c>
+      <c r="D50" s="9">
+        <f t="shared" si="1"/>
+        <v>1.4430303728851249E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B51" s="10">
+        <f t="shared" si="2"/>
         <v>30477.183233406937</v>
       </c>
-      <c r="C50" s="10">
-        <f t="shared" si="0"/>
-        <v>1.4537701572018696E-2</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B51" s="11">
-        <f t="shared" si="1"/>
+      <c r="C51" s="9">
+        <f t="shared" si="0"/>
+        <v>1.3172961549234748E-2</v>
+      </c>
+      <c r="D51" s="9">
+        <f t="shared" si="1"/>
+        <v>1.3172961549234802E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B52" s="10">
+        <f t="shared" si="2"/>
         <v>36572.619880088321</v>
       </c>
-      <c r="C51" s="10">
-        <f t="shared" si="0"/>
-        <v>1.3271008854247743E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B52" s="11">
-        <f t="shared" si="1"/>
+      <c r="C52" s="9">
+        <f t="shared" si="0"/>
+        <v>1.2025180768123598E-2</v>
+      </c>
+      <c r="D52" s="9">
+        <f t="shared" si="1"/>
+        <v>1.2025180768123646E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B53" s="10">
+        <f t="shared" si="2"/>
         <v>43887.143856105984</v>
       </c>
-      <c r="C52" s="10">
-        <f t="shared" si="0"/>
-        <v>1.2114690578957109E-2</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B53" s="11">
-        <f t="shared" si="1"/>
+      <c r="C53" s="9">
+        <f t="shared" si="0"/>
+        <v>1.0977412927820776E-2</v>
+      </c>
+      <c r="D53" s="9">
+        <f t="shared" si="1"/>
+        <v>1.0977412927820821E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B54" s="10">
+        <f t="shared" si="2"/>
         <v>52664.572627327179</v>
       </c>
-      <c r="C53" s="10">
-        <f t="shared" si="0"/>
-        <v>1.1059127845846051E-2</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B54" s="11">
-        <f t="shared" si="1"/>
+      <c r="C54" s="9">
+        <f t="shared" si="0"/>
+        <v>1.0020942111083115E-2</v>
+      </c>
+      <c r="D54" s="9">
+        <f t="shared" si="1"/>
+        <v>1.0020942111083155E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B55" s="10">
+        <f t="shared" si="2"/>
         <v>63197.487152792615</v>
       </c>
-      <c r="C54" s="10">
-        <f t="shared" si="0"/>
-        <v>1.0095540337623584E-2</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B55" s="11">
-        <f t="shared" si="1"/>
+      <c r="C55" s="9">
+        <f t="shared" si="0"/>
+        <v>9.1478122609306815E-3</v>
+      </c>
+      <c r="D55" s="9">
+        <f t="shared" si="1"/>
+        <v>9.147812260930718E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B56" s="10">
+        <f t="shared" si="2"/>
         <v>75836.984583351135</v>
       </c>
-      <c r="C55" s="10">
-        <f t="shared" si="0"/>
-        <v>9.2159131360812739E-3</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B56" s="11">
-        <f t="shared" si="1"/>
+      <c r="C56" s="9">
+        <f t="shared" si="0"/>
+        <v>8.3507608669276309E-3</v>
+      </c>
+      <c r="D56" s="9">
+        <f t="shared" si="1"/>
+        <v>8.3507608669276655E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B57" s="10">
+        <f t="shared" si="2"/>
         <v>91004.381500021365</v>
       </c>
-      <c r="C56" s="10">
-        <f t="shared" si="0"/>
-        <v>8.4129299430834789E-3</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B57" s="11"/>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B58" s="11"/>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B59" s="11"/>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B60" s="11"/>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B61" s="11"/>
+      <c r="C57" s="9">
+        <f t="shared" si="0"/>
+        <v>7.6231584551130329E-3</v>
+      </c>
+      <c r="D57" s="9">
+        <f t="shared" si="1"/>
+        <v>7.6231584551130632E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B58" s="10"/>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B59" s="10"/>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B60" s="10"/>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B61" s="10"/>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B62" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Excel with optimal exposure time
</commit_message>
<xml_diff>
--- a/Error_vs_Frame_vs_ExpPara.xlsx
+++ b/Error_vs_Frame_vs_ExpPara.xlsx
@@ -4,18 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="96" windowWidth="22116" windowHeight="9540" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="96" windowWidth="22116" windowHeight="9540" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
     <sheet name="min rel. error of D" sheetId="2" r:id="rId2"/>
+    <sheet name="CRLB for different t_exp" sheetId="3" r:id="rId3"/>
+    <sheet name="N-10000" sheetId="4" r:id="rId4"/>
+    <sheet name="N-10000_t_exp" sheetId="5" r:id="rId5"/>
+    <sheet name="N-10000_f" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="55">
   <si>
     <t>lambda [m]</t>
   </si>
@@ -239,17 +243,74 @@
   <si>
     <t>y2</t>
   </si>
+  <si>
+    <r>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[s]</t>
+    </r>
+  </si>
+  <si>
+    <t>Readout time</t>
+  </si>
+  <si>
+    <t>scale</t>
+  </si>
+  <si>
+    <t>scaling factor</t>
+  </si>
+  <si>
+    <t>original</t>
+  </si>
+  <si>
+    <t>f [Hz]</t>
+  </si>
+  <si>
+    <t>N = 20</t>
+  </si>
+  <si>
+    <t>N = 100</t>
+  </si>
+  <si>
+    <t>N = 500</t>
+  </si>
+  <si>
+    <t>N = 10000</t>
+  </si>
+  <si>
+    <t>N-fix</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0E+00"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="173" formatCode="0.0E+00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,8 +361,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,6 +386,18 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -328,12 +408,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -353,9 +434,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
+    <cellStyle name="Prozent" xfId="3" builtinId="5"/>
     <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -599,157 +699,157 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>0.76655347622849213</c:v>
+                  <c:v>0.76539982726438816</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.69337370792523434</c:v>
+                  <c:v>0.69233019317422118</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6282193556003236</c:v>
+                  <c:v>0.62727389695811098</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5699496770353456</c:v>
+                  <c:v>0.56909191319382169</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.51764752744540565</c:v>
+                  <c:v>0.51686847738258868</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.47056265164194316</c:v>
+                  <c:v>0.46985446345619036</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.42807193190244563</c:v>
+                  <c:v>0.42742769147289206</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.38965091757763648</c:v>
+                  <c:v>0.38906450007205384</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.35485304042240623</c:v>
+                  <c:v>0.35431899308560905</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.32329417523922777</c:v>
+                  <c:v>0.32280762341742841</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.2946409866702086</c:v>
+                  <c:v>0.29419755737323755</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.26860200186444427</c:v>
+                  <c:v>0.26819776076344271</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.24492067478164786</c:v>
+                  <c:v>0.24455207364485609</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.22336992540335199</c:v>
+                  <c:v>0.22303375775028567</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.20374778493048396</c:v>
+                  <c:v>0.20344114824000803</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.18587388015378753</c:v>
+                  <c:v>0.18559414336314842</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.1695865617652127</c:v>
+                  <c:v>0.1693313370909095</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.15474053222309928</c:v>
+                  <c:v>0.15450765055177426</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.1412048653257135</c:v>
+                  <c:v>0.1409923545855484</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.12886133618809978</c:v>
+                  <c:v>0.12866740223356618</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.1176029997776267</c:v>
+                  <c:v>0.11742600941351472</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.1073329705565106</c:v>
+                  <c:v>0.10717143639857299</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9.7963366509471655E-2</c:v>
+                  <c:v>9.7815933434287086E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>8.9414388893259825E-2</c:v>
+                  <c:v>8.9279821873056317E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8.1613515139824705E-2</c:v>
+                  <c:v>8.1490688291969038E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7.4494786986277151E-2</c:v>
+                  <c:v>7.4382673694115595E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>6.7998179462962563E-2</c:v>
+                  <c:v>6.7895843446323031E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6.2069039117141726E-2</c:v>
+                  <c:v>6.1975626348299132E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>5.665758198383803E-2</c:v>
+                  <c:v>5.6572313359024164E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5.1718443485569289E-2</c:v>
+                  <c:v>5.1640608173875502E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4.721027375943055E-2</c:v>
+                  <c:v>4.7139223160735724E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4.3095372956107665E-2</c:v>
+                  <c:v>4.3030515207874494E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.9339361893179554E-2</c:v>
+                  <c:v>3.9280156872911594E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.5910884121593496E-2</c:v>
+                  <c:v>3.5856838897676747E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.2781336015203111E-2</c:v>
+                  <c:v>3.2732000703957827E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.9924621945964437E-2</c:v>
+                  <c:v>2.987958593715391E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.7316931982616047E-2</c:v>
+                  <c:v>2.7275820499514703E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.4936539864415071E-2</c:v>
+                  <c:v>2.4899010827922455E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2.2763619266100415E-2</c:v>
+                  <c:v>2.2729360435373037E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2.0780076595263364E-2</c:v>
+                  <c:v>2.074880295998344E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.8969398756167408E-2</c:v>
+                  <c:v>1.894085015792427E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1.7316514480597893E-2</c:v>
+                  <c:v>1.7290453442963934E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1.5807667971123859E-2</c:v>
+                  <c:v>1.5783877719895055E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1.443030372885119E-2</c:v>
+                  <c:v>1.4408586385619765E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.3172961549234748E-2</c:v>
+                  <c:v>1.3153136482991195E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.2025180768123598E-2</c:v>
+                  <c:v>1.2007083090966663E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1.0977412927820776E-2</c:v>
+                  <c:v>1.0960892122103437E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.0020942111083115E-2</c:v>
+                  <c:v>1.0005860776454411E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>9.1478122609306815E-3</c:v>
+                  <c:v>9.134044970759923E-3</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>8.3507608669276309E-3</c:v>
+                  <c:v>8.3381931245295263E-3</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>7.6231584551130329E-3</c:v>
+                  <c:v>7.6116857410393696E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -764,11 +864,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="243197632"/>
-        <c:axId val="243198208"/>
+        <c:axId val="244386624"/>
+        <c:axId val="244387200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="243197632"/>
+        <c:axId val="244386624"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -805,12 +905,12 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="243198208"/>
+        <c:crossAx val="244387200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="243198208"/>
+        <c:axId val="244387200"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -845,7 +945,7 @@
         <c:spPr>
           <a:ln w="9525"/>
         </c:spPr>
-        <c:crossAx val="243197632"/>
+        <c:crossAx val="244386624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -865,6 +965,848 @@
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'CRLB for different t_exp'!$Q$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CRLB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'CRLB for different t_exp'!$P$9:$P$30</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19841.268864953439</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19841.266753886615</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19841.260078110121</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19841.238967480815</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19841.172210105</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19840.961107703162</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19840.293572855939</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19838.182937897764</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19831.511478478846</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19810.44397053037</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19744.1162533565</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>19537.261959039406</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18910.741301059003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17169.607804706429</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13297.872340425529</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7762.4994383131861</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3351.206434316352</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1198.1143696653987</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>395.1944356623456</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>126.69696975468695</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40.240800952902127</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'CRLB for different t_exp'!$Q$9:$Q$30</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>2.2963143003787198E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.8955880948354286E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.4788503212630039E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4424903297775374E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.7072410187041481E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2213078003562148E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9428453965869005E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.8134081357731698E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7639883994937731E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.7473612482116031E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.7426133171558531E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.7431420958895105E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.7497499696060136E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.7719834373656904E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.8406020433312568E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.0398977551644208E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.5591666434572197E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.7340091112431854E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.0934358738225301E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.1051081409931628</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.18547505790524033</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.3315699565126673</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="212876032"/>
+        <c:axId val="39890880"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="212876032"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>u</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="high"/>
+        <c:crossAx val="39890880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="39890880"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>rel. Error CRLB</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="212876032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'CRLB for different t_exp'!$B$10:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>0.0E+00</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>9.9999999999999994E-12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1622776601683794E-11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1E-10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1622776601683795E-10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0000000000000001E-9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.1622776601683795E-9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0000000000000002E-8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.1622776601683799E-8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0000000000000002E-7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.1622776601683802E-7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0000000000000004E-6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.1622776601683809E-6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.0000000000000006E-5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.1622776601683816E-5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0000000000000007E-4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.1622776601683816E-4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.0000000000000007E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.1622776601683816E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.1622776601683819E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.10000000000000009</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'CRLB for different t_exp'!$Q$10:$Q$30</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>5.8955880948354286E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.4788503212630039E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.4424903297775374E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7072410187041481E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2213078003562148E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9428453965869005E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8134081357731698E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7639883994937731E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7473612482116031E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.7426133171558531E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.7431420958895105E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.7497499696060136E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.7719834373656904E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.8406020433312568E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.0398977551644208E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.5591666434572197E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.7340091112431854E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.0934358738225301E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.1051081409931628</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.18547505790524033</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.3315699565126673</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="39893184"/>
+        <c:axId val="148725760"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="39893184"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>t_exp [s]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.0E+00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:crossAx val="148725760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="148725760"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>rel. Error of Diameter (CRLB)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:crossAx val="39893184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'CRLB for different t_exp'!$D$10:$D$30</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>4920.6346785084525</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4920.6341549638801</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4920.6324993713097</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4920.6272639352419</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4920.61070810604</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4920.5583547103843</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4920.3928060682729</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4919.8693685986455</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4918.2148466627532</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4912.990104691532</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4896.5408308324122</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4845.2409658417728</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4689.863842662633</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4258.0627355671941</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3297.8723404255311</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1925.0998607016702</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>831.09919571045521</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>297.13236367701887</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>98.008220044261705</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>31.420848499162364</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.9797186363197277</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'CRLB for different t_exp'!$Q$10:$Q$30</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>5.8955880948354286E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.4788503212630039E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.4424903297775374E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7072410187041481E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2213078003562148E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9428453965869005E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8134081357731698E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7639883994937731E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7473612482116031E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.7426133171558531E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.7431420958895105E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.7497499696060136E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.7719834373656904E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.8406020433312568E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.0398977551644208E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.5591666434572197E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.7340091112431854E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.0934358738225301E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.1051081409931628</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.18547505790524033</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.3315699565126673</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="153751488"/>
+        <c:axId val="153752064"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="153751488"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>framerate [Hz]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:crossAx val="153752064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="153752064"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>rel. Error of Diameter (CRLB)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:crossAx val="153751488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="98" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="90" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -899,6 +1841,87 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9291735" cy="6002694"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9291735" cy="6002694"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9291735" cy="6002694"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1189,10 +2212,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F25"/>
+  <dimension ref="B1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1373,119 +2396,136 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B17" s="12"/>
       <c r="C17" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="2">
+        <f>E16-E14</f>
+        <v>2.0322580645161289E-4</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="12"/>
+      <c r="C18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E18" s="5">
         <f>1/6*E14/E16</f>
         <v>8.2666666666666666E-2</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="12"/>
-      <c r="C18" s="3" t="s">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="12"/>
+      <c r="C19" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D19" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="5">
-        <v>1000</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="E19" s="5">
+        <v>787122</v>
+      </c>
+      <c r="F19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D19" s="7"/>
-    </row>
-    <row r="20" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="B20" s="12" t="s">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="2:7" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="B21" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="1">
-        <f>E4/SQRT(E18)</f>
-        <v>2.8263172815520908E-9</v>
-      </c>
-      <c r="F20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="12"/>
       <c r="C21" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E21" s="1">
-        <f>E20*SQRT(1+E11*E14/(E4^2))</f>
-        <v>3.0689984289079374E-9</v>
+        <f>E4/SQRT(E19)</f>
+        <v>1.0073952261491022E-10</v>
       </c>
       <c r="F21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="12"/>
       <c r="C22" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="1">
+        <f>E21*SQRT(1+E11*E14/(E4^2))</f>
+        <v>1.0938950083633663E-10</v>
+      </c>
+      <c r="F22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="12"/>
+      <c r="C23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="1">
-        <f>E20^2/(E11*E16)*(1+E11*E14/(E4^2))-1/3*E14/E16</f>
-        <v>-0.16206796707017168</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="E23" s="1">
+        <f>E22^2/(E11*E16)-2*E18</f>
+        <v>-0.16532918484521691</v>
+      </c>
+      <c r="F23" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="12"/>
-      <c r="E23" s="8" t="str">
-        <f>IF(E22&lt;(2/3)," quasi optimal fit possible", "not optimal fit possible")</f>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="12"/>
+      <c r="E24" s="8" t="str">
+        <f>IF(E23&lt;(2/3)," quasi optimal fit possible", "not optimal fit possible")</f>
         <v xml:space="preserve"> quasi optimal fit possible</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="B24" s="12"/>
-      <c r="C24" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="1">
-        <f>1+E4^2/(E11*E16)</f>
-        <v>3.7693662631616411</v>
-      </c>
-      <c r="F24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B25" s="12"/>
       <c r="C25" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="1">
+        <f>1+E4^2/(E11*E16)</f>
+        <v>3.7693662631616411</v>
+      </c>
+      <c r="F25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="12"/>
+      <c r="C26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1493,11 +2533,11 @@
   <mergeCells count="4">
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B7:B11"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="B21:B26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1505,8 +2545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1520,15 +2560,15 @@
         <v>29</v>
       </c>
       <c r="C2" s="6">
-        <f>Inputs!E22</f>
-        <v>-0.16206796707017168</v>
+        <f>Inputs!E23</f>
+        <v>-0.16532918484521691</v>
       </c>
       <c r="E2" t="s">
         <v>42</v>
       </c>
       <c r="F2" s="11">
         <f>1/SQRT(1+2*$C$2)</f>
-        <v>1.216382943469255</v>
+        <v>1.2222951300196552</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
@@ -1543,7 +2583,7 @@
       </c>
       <c r="F3" s="11">
         <f>(1+$C$2)/((1+2*$C$2)^(3/2))</f>
-        <v>1.5080639497321757</v>
+        <v>1.5242053180845554</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
@@ -1552,7 +2592,7 @@
       </c>
       <c r="F4" s="11">
         <f>(1-F2)/SQRT(F3-(F2)^2)</f>
-        <v>-1.282271049205649</v>
+        <v>-1.2791661463991237</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
@@ -1580,11 +2620,11 @@
       </c>
       <c r="C7" s="9">
         <f>SQRT(2/(B7-1)*(1+2*SQRT(1+2*$C$2)))</f>
-        <v>0.76655347622849213</v>
+        <v>0.76539982726438816</v>
       </c>
       <c r="D7" s="9">
         <f>SQRT(2/(B7-1)*(1+$F$4^2))</f>
-        <v>0.76655347622849523</v>
+        <v>0.76539982726438616</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
@@ -1594,11 +2634,11 @@
       </c>
       <c r="C8" s="9">
         <f t="shared" ref="C8:C57" si="0">SQRT(2/(B8-1)*(1+2*SQRT(1+2*$C$2)))</f>
-        <v>0.69337370792523434</v>
+        <v>0.69233019317422118</v>
       </c>
       <c r="D8" s="9">
         <f t="shared" ref="D8:D57" si="1">SQRT(2/(B8-1)*(1+$F$4^2))</f>
-        <v>0.69337370792523711</v>
+        <v>0.69233019317421929</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
@@ -1608,11 +2648,11 @@
       </c>
       <c r="C9" s="9">
         <f t="shared" si="0"/>
-        <v>0.6282193556003236</v>
+        <v>0.62727389695811098</v>
       </c>
       <c r="D9" s="9">
         <f t="shared" si="1"/>
-        <v>0.62821935560032616</v>
+        <v>0.62727389695810931</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
@@ -1622,11 +2662,11 @@
       </c>
       <c r="C10" s="9">
         <f t="shared" si="0"/>
-        <v>0.5699496770353456</v>
+        <v>0.56909191319382169</v>
       </c>
       <c r="D10" s="9">
         <f t="shared" si="1"/>
-        <v>0.56994967703534793</v>
+        <v>0.56909191319382024</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
@@ -1636,11 +2676,11 @@
       </c>
       <c r="C11" s="9">
         <f t="shared" si="0"/>
-        <v>0.51764752744540565</v>
+        <v>0.51686847738258868</v>
       </c>
       <c r="D11" s="9">
         <f t="shared" si="1"/>
-        <v>0.51764752744540776</v>
+        <v>0.51686847738258734</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
@@ -1650,11 +2690,11 @@
       </c>
       <c r="C12" s="9">
         <f t="shared" si="0"/>
-        <v>0.47056265164194316</v>
+        <v>0.46985446345619036</v>
       </c>
       <c r="D12" s="9">
         <f t="shared" si="1"/>
-        <v>0.47056265164194505</v>
+        <v>0.46985446345618909</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
@@ -1664,11 +2704,11 @@
       </c>
       <c r="C13" s="9">
         <f t="shared" si="0"/>
-        <v>0.42807193190244563</v>
+        <v>0.42742769147289206</v>
       </c>
       <c r="D13" s="9">
         <f t="shared" si="1"/>
-        <v>0.42807193190244736</v>
+        <v>0.42742769147289084</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
@@ -1678,11 +2718,11 @@
       </c>
       <c r="C14" s="9">
         <f t="shared" si="0"/>
-        <v>0.38965091757763648</v>
+        <v>0.38906450007205384</v>
       </c>
       <c r="D14" s="9">
         <f t="shared" si="1"/>
-        <v>0.38965091757763809</v>
+        <v>0.38906450007205279</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
@@ -1692,11 +2732,11 @@
       </c>
       <c r="C15" s="9">
         <f t="shared" si="0"/>
-        <v>0.35485304042240623</v>
+        <v>0.35431899308560905</v>
       </c>
       <c r="D15" s="9">
         <f t="shared" si="1"/>
-        <v>0.35485304042240767</v>
+        <v>0.3543189930856081</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
@@ -1706,11 +2746,11 @@
       </c>
       <c r="C16" s="9">
         <f t="shared" si="0"/>
-        <v>0.32329417523922777</v>
+        <v>0.32280762341742841</v>
       </c>
       <c r="D16" s="9">
         <f t="shared" si="1"/>
-        <v>0.32329417523922904</v>
+        <v>0.32280762341742752</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
@@ -1720,11 +2760,11 @@
       </c>
       <c r="C17" s="9">
         <f t="shared" si="0"/>
-        <v>0.2946409866702086</v>
+        <v>0.29419755737323755</v>
       </c>
       <c r="D17" s="9">
         <f t="shared" si="1"/>
-        <v>0.29464098667020977</v>
+        <v>0.29419755737323677</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
@@ -1734,11 +2774,11 @@
       </c>
       <c r="C18" s="9">
         <f t="shared" si="0"/>
-        <v>0.26860200186444427</v>
+        <v>0.26819776076344271</v>
       </c>
       <c r="D18" s="9">
         <f t="shared" si="1"/>
-        <v>0.26860200186444538</v>
+        <v>0.26819776076344198</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
@@ -1748,11 +2788,11 @@
       </c>
       <c r="C19" s="9">
         <f t="shared" si="0"/>
-        <v>0.24492067478164786</v>
+        <v>0.24455207364485609</v>
       </c>
       <c r="D19" s="9">
         <f t="shared" si="1"/>
-        <v>0.24492067478164886</v>
+        <v>0.24455207364485543</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
@@ -1762,11 +2802,11 @@
       </c>
       <c r="C20" s="9">
         <f t="shared" si="0"/>
-        <v>0.22336992540335199</v>
+        <v>0.22303375775028567</v>
       </c>
       <c r="D20" s="9">
         <f t="shared" si="1"/>
-        <v>0.22336992540335288</v>
+        <v>0.22303375775028506</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
@@ -1776,11 +2816,11 @@
       </c>
       <c r="C21" s="9">
         <f t="shared" si="0"/>
-        <v>0.20374778493048396</v>
+        <v>0.20344114824000803</v>
       </c>
       <c r="D21" s="9">
         <f t="shared" si="1"/>
-        <v>0.20374778493048479</v>
+        <v>0.20344114824000745</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
@@ -1790,11 +2830,11 @@
       </c>
       <c r="C22" s="9">
         <f t="shared" si="0"/>
-        <v>0.18587388015378753</v>
+        <v>0.18559414336314842</v>
       </c>
       <c r="D22" s="9">
         <f t="shared" si="1"/>
-        <v>0.18587388015378828</v>
+        <v>0.18559414336314792</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
@@ -1804,11 +2844,11 @@
       </c>
       <c r="C23" s="9">
         <f t="shared" si="0"/>
-        <v>0.1695865617652127</v>
+        <v>0.1693313370909095</v>
       </c>
       <c r="D23" s="9">
         <f t="shared" si="1"/>
-        <v>0.16958656176521339</v>
+        <v>0.16933133709090906</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
@@ -1818,11 +2858,11 @@
       </c>
       <c r="C24" s="9">
         <f t="shared" si="0"/>
-        <v>0.15474053222309928</v>
+        <v>0.15450765055177426</v>
       </c>
       <c r="D24" s="9">
         <f t="shared" si="1"/>
-        <v>0.15474053222309991</v>
+        <v>0.15450765055177385</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
@@ -1832,11 +2872,11 @@
       </c>
       <c r="C25" s="9">
         <f t="shared" si="0"/>
-        <v>0.1412048653257135</v>
+        <v>0.1409923545855484</v>
       </c>
       <c r="D25" s="9">
         <f t="shared" si="1"/>
-        <v>0.14120486532571408</v>
+        <v>0.14099235458554801</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
@@ -1846,11 +2886,11 @@
       </c>
       <c r="C26" s="9">
         <f t="shared" si="0"/>
-        <v>0.12886133618809978</v>
+        <v>0.12866740223356618</v>
       </c>
       <c r="D26" s="9">
         <f t="shared" si="1"/>
-        <v>0.12886133618810028</v>
+        <v>0.12866740223356585</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
@@ -1860,11 +2900,11 @@
       </c>
       <c r="C27" s="9">
         <f t="shared" si="0"/>
-        <v>0.1176029997776267</v>
+        <v>0.11742600941351472</v>
       </c>
       <c r="D27" s="9">
         <f t="shared" si="1"/>
-        <v>0.11760299977762717</v>
+        <v>0.1174260094135144</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
@@ -1874,11 +2914,11 @@
       </c>
       <c r="C28" s="9">
         <f t="shared" si="0"/>
-        <v>0.1073329705565106</v>
+        <v>0.10717143639857299</v>
       </c>
       <c r="D28" s="9">
         <f t="shared" si="1"/>
-        <v>0.10733297055651105</v>
+        <v>0.1071714363985727</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.3">
@@ -1888,11 +2928,11 @@
       </c>
       <c r="C29" s="9">
         <f t="shared" si="0"/>
-        <v>9.7963366509471655E-2</v>
+        <v>9.7815933434287086E-2</v>
       </c>
       <c r="D29" s="9">
         <f t="shared" si="1"/>
-        <v>9.7963366509472044E-2</v>
+        <v>9.7815933434286823E-2</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
@@ -1902,11 +2942,11 @@
       </c>
       <c r="C30" s="9">
         <f t="shared" si="0"/>
-        <v>8.9414388893259825E-2</v>
+        <v>8.9279821873056317E-2</v>
       </c>
       <c r="D30" s="9">
         <f t="shared" si="1"/>
-        <v>8.9414388893260172E-2</v>
+        <v>8.9279821873056081E-2</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
@@ -1916,11 +2956,11 @@
       </c>
       <c r="C31" s="9">
         <f t="shared" si="0"/>
-        <v>8.1613515139824705E-2</v>
+        <v>8.1490688291969038E-2</v>
       </c>
       <c r="D31" s="9">
         <f t="shared" si="1"/>
-        <v>8.1613515139825038E-2</v>
+        <v>8.149068829196883E-2</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
@@ -1930,11 +2970,11 @@
       </c>
       <c r="C32" s="9">
         <f t="shared" si="0"/>
-        <v>7.4494786986277151E-2</v>
+        <v>7.4382673694115595E-2</v>
       </c>
       <c r="D32" s="9">
         <f t="shared" si="1"/>
-        <v>7.4494786986277456E-2</v>
+        <v>7.4382673694115387E-2</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
@@ -1944,11 +2984,11 @@
       </c>
       <c r="C33" s="9">
         <f t="shared" si="0"/>
-        <v>6.7998179462962563E-2</v>
+        <v>6.7895843446323031E-2</v>
       </c>
       <c r="D33" s="9">
         <f t="shared" si="1"/>
-        <v>6.7998179462962827E-2</v>
+        <v>6.7895843446322851E-2</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
@@ -1958,11 +2998,11 @@
       </c>
       <c r="C34" s="9">
         <f t="shared" si="0"/>
-        <v>6.2069039117141726E-2</v>
+        <v>6.1975626348299132E-2</v>
       </c>
       <c r="D34" s="9">
         <f t="shared" si="1"/>
-        <v>6.2069039117141976E-2</v>
+        <v>6.1975626348298958E-2</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
@@ -1972,11 +3012,11 @@
       </c>
       <c r="C35" s="9">
         <f t="shared" si="0"/>
-        <v>5.665758198383803E-2</v>
+        <v>5.6572313359024164E-2</v>
       </c>
       <c r="D35" s="9">
         <f t="shared" si="1"/>
-        <v>5.6657581983838259E-2</v>
+        <v>5.6572313359024018E-2</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
@@ -1986,11 +3026,11 @@
       </c>
       <c r="C36" s="9">
         <f t="shared" si="0"/>
-        <v>5.1718443485569289E-2</v>
+        <v>5.1640608173875502E-2</v>
       </c>
       <c r="D36" s="9">
         <f t="shared" si="1"/>
-        <v>5.171844348556949E-2</v>
+        <v>5.1640608173875363E-2</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
@@ -2000,11 +3040,11 @@
       </c>
       <c r="C37" s="9">
         <f t="shared" si="0"/>
-        <v>4.721027375943055E-2</v>
+        <v>4.7139223160735724E-2</v>
       </c>
       <c r="D37" s="9">
         <f t="shared" si="1"/>
-        <v>4.7210273759430738E-2</v>
+        <v>4.7139223160735592E-2</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
@@ -2014,11 +3054,11 @@
       </c>
       <c r="C38" s="9">
         <f t="shared" si="0"/>
-        <v>4.3095372956107665E-2</v>
+        <v>4.3030515207874494E-2</v>
       </c>
       <c r="D38" s="9">
         <f t="shared" si="1"/>
-        <v>4.3095372956107839E-2</v>
+        <v>4.3030515207874376E-2</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
@@ -2028,11 +3068,11 @@
       </c>
       <c r="C39" s="9">
         <f t="shared" si="0"/>
-        <v>3.9339361893179554E-2</v>
+        <v>3.9280156872911594E-2</v>
       </c>
       <c r="D39" s="9">
         <f t="shared" si="1"/>
-        <v>3.9339361893179714E-2</v>
+        <v>3.928015687291149E-2</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
@@ -2042,11 +3082,11 @@
       </c>
       <c r="C40" s="9">
         <f t="shared" si="0"/>
-        <v>3.5910884121593496E-2</v>
+        <v>3.5856838897676747E-2</v>
       </c>
       <c r="D40" s="9">
         <f t="shared" si="1"/>
-        <v>3.5910884121593642E-2</v>
+        <v>3.585683889767665E-2</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
@@ -2056,11 +3096,11 @@
       </c>
       <c r="C41" s="9">
         <f t="shared" si="0"/>
-        <v>3.2781336015203111E-2</v>
+        <v>3.2732000703957827E-2</v>
       </c>
       <c r="D41" s="9">
         <f t="shared" si="1"/>
-        <v>3.2781336015203236E-2</v>
+        <v>3.2732000703957737E-2</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
@@ -2070,11 +3110,11 @@
       </c>
       <c r="C42" s="9">
         <f t="shared" si="0"/>
-        <v>2.9924621945964437E-2</v>
+        <v>2.987958593715391E-2</v>
       </c>
       <c r="D42" s="9">
         <f t="shared" si="1"/>
-        <v>2.9924621945964555E-2</v>
+        <v>2.987958593715383E-2</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
@@ -2084,11 +3124,11 @@
       </c>
       <c r="C43" s="9">
         <f t="shared" si="0"/>
-        <v>2.7316931982616047E-2</v>
+        <v>2.7275820499514703E-2</v>
       </c>
       <c r="D43" s="9">
         <f t="shared" si="1"/>
-        <v>2.7316931982616158E-2</v>
+        <v>2.7275820499514627E-2</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
@@ -2098,11 +3138,11 @@
       </c>
       <c r="C44" s="9">
         <f t="shared" si="0"/>
-        <v>2.4936539864415071E-2</v>
+        <v>2.4899010827922455E-2</v>
       </c>
       <c r="D44" s="9">
         <f t="shared" si="1"/>
-        <v>2.4936539864415172E-2</v>
+        <v>2.489901082792239E-2</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
@@ -2112,11 +3152,11 @@
       </c>
       <c r="C45" s="9">
         <f t="shared" si="0"/>
-        <v>2.2763619266100415E-2</v>
+        <v>2.2729360435373037E-2</v>
       </c>
       <c r="D45" s="9">
         <f t="shared" si="1"/>
-        <v>2.2763619266100505E-2</v>
+        <v>2.2729360435372978E-2</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
@@ -2126,11 +3166,11 @@
       </c>
       <c r="C46" s="9">
         <f t="shared" si="0"/>
-        <v>2.0780076595263364E-2</v>
+        <v>2.074880295998344E-2</v>
       </c>
       <c r="D46" s="9">
         <f t="shared" si="1"/>
-        <v>2.0780076595263451E-2</v>
+        <v>2.0748802959983388E-2</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
@@ -2140,11 +3180,11 @@
       </c>
       <c r="C47" s="9">
         <f t="shared" si="0"/>
-        <v>1.8969398756167408E-2</v>
+        <v>1.894085015792427E-2</v>
       </c>
       <c r="D47" s="9">
         <f t="shared" si="1"/>
-        <v>1.8969398756167485E-2</v>
+        <v>1.8940850157924221E-2</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
@@ -2154,11 +3194,11 @@
       </c>
       <c r="C48" s="9">
         <f t="shared" si="0"/>
-        <v>1.7316514480597893E-2</v>
+        <v>1.7290453442963934E-2</v>
       </c>
       <c r="D48" s="9">
         <f t="shared" si="1"/>
-        <v>1.7316514480597966E-2</v>
+        <v>1.7290453442963889E-2</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
@@ -2168,11 +3208,11 @@
       </c>
       <c r="C49" s="9">
         <f t="shared" si="0"/>
-        <v>1.5807667971123859E-2</v>
+        <v>1.5783877719895055E-2</v>
       </c>
       <c r="D49" s="9">
         <f t="shared" si="1"/>
-        <v>1.5807667971123922E-2</v>
+        <v>1.5783877719895017E-2</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
@@ -2182,11 +3222,11 @@
       </c>
       <c r="C50" s="9">
         <f t="shared" si="0"/>
-        <v>1.443030372885119E-2</v>
+        <v>1.4408586385619765E-2</v>
       </c>
       <c r="D50" s="9">
         <f t="shared" si="1"/>
-        <v>1.4430303728851249E-2</v>
+        <v>1.4408586385619726E-2</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
@@ -2196,11 +3236,11 @@
       </c>
       <c r="C51" s="9">
         <f t="shared" si="0"/>
-        <v>1.3172961549234748E-2</v>
+        <v>1.3153136482991195E-2</v>
       </c>
       <c r="D51" s="9">
         <f t="shared" si="1"/>
-        <v>1.3172961549234802E-2</v>
+        <v>1.315313648299116E-2</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.3">
@@ -2210,11 +3250,11 @@
       </c>
       <c r="C52" s="9">
         <f t="shared" si="0"/>
-        <v>1.2025180768123598E-2</v>
+        <v>1.2007083090966663E-2</v>
       </c>
       <c r="D52" s="9">
         <f t="shared" si="1"/>
-        <v>1.2025180768123646E-2</v>
+        <v>1.200708309096663E-2</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.3">
@@ -2224,11 +3264,11 @@
       </c>
       <c r="C53" s="9">
         <f t="shared" si="0"/>
-        <v>1.0977412927820776E-2</v>
+        <v>1.0960892122103437E-2</v>
       </c>
       <c r="D53" s="9">
         <f t="shared" si="1"/>
-        <v>1.0977412927820821E-2</v>
+        <v>1.0960892122103407E-2</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.3">
@@ -2238,11 +3278,11 @@
       </c>
       <c r="C54" s="9">
         <f t="shared" si="0"/>
-        <v>1.0020942111083115E-2</v>
+        <v>1.0005860776454411E-2</v>
       </c>
       <c r="D54" s="9">
         <f t="shared" si="1"/>
-        <v>1.0020942111083155E-2</v>
+        <v>1.0005860776454384E-2</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.3">
@@ -2252,11 +3292,11 @@
       </c>
       <c r="C55" s="9">
         <f t="shared" si="0"/>
-        <v>9.1478122609306815E-3</v>
+        <v>9.134044970759923E-3</v>
       </c>
       <c r="D55" s="9">
         <f t="shared" si="1"/>
-        <v>9.147812260930718E-3</v>
+        <v>9.1340449707598987E-3</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.3">
@@ -2266,11 +3306,11 @@
       </c>
       <c r="C56" s="9">
         <f t="shared" si="0"/>
-        <v>8.3507608669276309E-3</v>
+        <v>8.3381931245295263E-3</v>
       </c>
       <c r="D56" s="9">
         <f t="shared" si="1"/>
-        <v>8.3507608669276655E-3</v>
+        <v>8.3381931245295037E-3</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.3">
@@ -2280,11 +3320,11 @@
       </c>
       <c r="C57" s="9">
         <f t="shared" si="0"/>
-        <v>7.6231584551130329E-3</v>
+        <v>7.6116857410393696E-3</v>
       </c>
       <c r="D57" s="9">
         <f t="shared" si="1"/>
-        <v>7.6231584551130632E-3</v>
+        <v>7.6116857410393497E-3</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.3">
@@ -2307,4 +3347,1888 @@
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" style="13"/>
+    <col min="2" max="3" width="11.5546875" style="1"/>
+    <col min="4" max="4" width="11.5546875" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="1">
+        <f>10^(1/2)</f>
+        <v>3.1622776601683795</v>
+      </c>
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1">
+        <f>Inputs!E14</f>
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2">
+        <f>Inputs!E17</f>
+        <v>2.0322580645161289E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3">
+        <f>Inputs!E19</f>
+        <v>787122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="1">
+        <f>Inputs!$E$4</f>
+        <v>8.9376000000000006E-8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1">
+        <f>Inputs!E11</f>
+        <v>7.1534099031969463E-12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="J7" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="S7" s="24"/>
+    </row>
+    <row r="8" spans="1:19" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A8" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="R8" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="S8" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14">
+        <v>1</v>
+      </c>
+      <c r="B9" s="25">
+        <f>H1</f>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C9" s="17">
+        <f>B9+$H$2</f>
+        <v>4.032258064516129E-4</v>
+      </c>
+      <c r="D9" s="20">
+        <f>1/C9</f>
+        <v>2480</v>
+      </c>
+      <c r="E9" s="20">
+        <f>H3</f>
+        <v>787122</v>
+      </c>
+      <c r="F9" s="17">
+        <f>$H$4/SQRT(E9)</f>
+        <v>1.0073952261491022E-10</v>
+      </c>
+      <c r="G9" s="17">
+        <f>F9*SQRT(1+$H$5*B9/($H$4^2))</f>
+        <v>1.0938950083633663E-10</v>
+      </c>
+      <c r="H9" s="16">
+        <f>1/6*B9/C9</f>
+        <v>8.2666666666666666E-2</v>
+      </c>
+      <c r="I9" s="17">
+        <f>G9^2/($H$5*C9)-2*H9</f>
+        <v>-0.16532918484521691</v>
+      </c>
+      <c r="J9" s="15">
+        <v>20</v>
+      </c>
+      <c r="K9" s="27">
+        <f>1/SQRT(J9-1)*SQRT(2*(1+2*SQRT(1+2*$I9)))</f>
+        <v>0.5267842892287824</v>
+      </c>
+      <c r="L9" s="15">
+        <v>100</v>
+      </c>
+      <c r="M9" s="27">
+        <f>1/SQRT(L9-1)*SQRT(2*(1+2*SQRT(1+2*$I9)))</f>
+        <v>0.2307767310580737</v>
+      </c>
+      <c r="N9" s="15">
+        <v>500</v>
+      </c>
+      <c r="O9" s="27">
+        <f>1/SQRT(N9-1)*SQRT(2*(1+2*SQRT(1+2*$I9)))</f>
+        <v>0.10279200607732683</v>
+      </c>
+      <c r="P9" s="15">
+        <v>10000</v>
+      </c>
+      <c r="Q9" s="27">
+        <f>1/SQRT(P9-1)*SQRT(2*(1+2*SQRT(1+2*$I9)))</f>
+        <v>2.2963143003787198E-2</v>
+      </c>
+      <c r="R9" s="15">
+        <v>1000</v>
+      </c>
+      <c r="S9" s="27">
+        <f>1/SQRT(R9-1)*SQRT(2*(1+2*SQRT(1+2*$I9)))</f>
+        <v>7.2648536599557556E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" s="13">
+        <f>B10/$B$9</f>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="B10" s="26">
+        <v>9.9999999999999994E-12</v>
+      </c>
+      <c r="C10" s="18">
+        <f>B10+$H$2</f>
+        <v>2.0322581645161288E-4</v>
+      </c>
+      <c r="D10" s="21">
+        <f>1/C10</f>
+        <v>4920.6346785084525</v>
+      </c>
+      <c r="E10" s="21">
+        <f>$E$9*A10</f>
+        <v>3.9356099999999998E-2</v>
+      </c>
+      <c r="F10" s="18">
+        <f>$H$4/SQRT(E10)</f>
+        <v>4.5052084117563325E-7</v>
+      </c>
+      <c r="G10" s="18">
+        <f>F10*SQRT(1+$H$5*B10/($H$4^2))</f>
+        <v>4.5052084319286668E-7</v>
+      </c>
+      <c r="H10" s="23">
+        <f t="shared" ref="H10:H25" si="0">1/6*B10/C10</f>
+        <v>8.2010577975140877E-9</v>
+      </c>
+      <c r="I10" s="18">
+        <f>G10^2/($H$5*C10)-2*H10</f>
+        <v>139.61683474360959</v>
+      </c>
+      <c r="J10" s="21">
+        <f>J$9*$C$9/$C10</f>
+        <v>39.682537729906876</v>
+      </c>
+      <c r="K10" s="28">
+        <f t="shared" ref="K10:K30" si="1">1/SQRT(J10-1)*SQRT(2*(1+2*SQRT(1+2*$I10)))</f>
+        <v>1.3351911064236686</v>
+      </c>
+      <c r="L10" s="21">
+        <f>L$9*$C$9/$C10</f>
+        <v>198.41268864953437</v>
+      </c>
+      <c r="M10" s="28">
+        <f t="shared" ref="M10:M30" si="2">1/SQRT(L10-1)*SQRT(2*(1+2*SQRT(1+2*$I10)))</f>
+        <v>0.59103524269790697</v>
+      </c>
+      <c r="N10" s="21">
+        <f>N$9*$C$9/$C10</f>
+        <v>992.0634432476719</v>
+      </c>
+      <c r="O10" s="28">
+        <f t="shared" ref="O10:O30" si="3">1/SQRT(N10-1)*SQRT(2*(1+2*SQRT(1+2*$I10)))</f>
+        <v>0.26378505185653606</v>
+      </c>
+      <c r="P10" s="21">
+        <f>P$9*$C$9/$C10</f>
+        <v>19841.268864953439</v>
+      </c>
+      <c r="Q10" s="28">
+        <f t="shared" ref="Q10:S30" si="4">1/SQRT(P10-1)*SQRT(2*(1+2*SQRT(1+2*$I10)))</f>
+        <v>5.8955880948354286E-2</v>
+      </c>
+      <c r="R10" s="21">
+        <f>R9</f>
+        <v>1000</v>
+      </c>
+      <c r="S10" s="28">
+        <f t="shared" si="4"/>
+        <v>0.26273514210852766</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="13">
+        <f t="shared" ref="A11:A30" si="5">B11/$B$9</f>
+        <v>1.5811388300841896E-7</v>
+      </c>
+      <c r="B11" s="26">
+        <f>$B$1*B10</f>
+        <v>3.1622776601683794E-11</v>
+      </c>
+      <c r="C11" s="18">
+        <f t="shared" ref="C11:C30" si="6">B11+$H$2</f>
+        <v>2.032258380743895E-4</v>
+      </c>
+      <c r="D11" s="21">
+        <f t="shared" ref="D11:D30" si="7">1/C11</f>
+        <v>4920.6341549638801</v>
+      </c>
+      <c r="E11" s="21">
+        <f>$E$9*A11</f>
+        <v>0.12445491582135275</v>
+      </c>
+      <c r="F11" s="18">
+        <f t="shared" ref="F10:F30" si="8">$H$4/SQRT(E11)</f>
+        <v>2.5334648685257639E-7</v>
+      </c>
+      <c r="G11" s="18">
+        <f>F11*SQRT(1+$H$5*B11/($H$4^2))</f>
+        <v>2.533464904397812E-7</v>
+      </c>
+      <c r="H11" s="23">
+        <f t="shared" si="0"/>
+        <v>2.5934019103506316E-8</v>
+      </c>
+      <c r="I11" s="18">
+        <f t="shared" ref="I11:I25" si="9">G11^2/($H$5*C11)-2*H11</f>
+        <v>44.150715860004397</v>
+      </c>
+      <c r="J11" s="21">
+        <f>J$9*$C$9/$C11</f>
+        <v>39.682533507773229</v>
+      </c>
+      <c r="K11" s="28">
+        <f t="shared" si="1"/>
+        <v>1.0143383540312148</v>
+      </c>
+      <c r="L11" s="21">
+        <f>L$9*$C$9/$C11</f>
+        <v>198.41266753886615</v>
+      </c>
+      <c r="M11" s="28">
+        <f t="shared" si="2"/>
+        <v>0.44900667155842605</v>
+      </c>
+      <c r="N11" s="21">
+        <f>N$9*$C$9/$C11</f>
+        <v>992.0633376943307</v>
+      </c>
+      <c r="O11" s="28">
+        <f t="shared" si="3"/>
+        <v>0.20039625314855972</v>
+      </c>
+      <c r="P11" s="21">
+        <f>P$9*$C$9/$C11</f>
+        <v>19841.266753886615</v>
+      </c>
+      <c r="Q11" s="28">
+        <f t="shared" si="4"/>
+        <v>4.4788503212630039E-2</v>
+      </c>
+      <c r="R11" s="21">
+        <f t="shared" ref="R11:R30" si="10">R10</f>
+        <v>1000</v>
+      </c>
+      <c r="S11" s="28">
+        <f t="shared" si="4"/>
+        <v>0.19959863106204476</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" s="13">
+        <f t="shared" si="5"/>
+        <v>4.9999999999999998E-7</v>
+      </c>
+      <c r="B12" s="26">
+        <f t="shared" ref="B12:B30" si="11">$B$1*B11</f>
+        <v>1E-10</v>
+      </c>
+      <c r="C12" s="18">
+        <f t="shared" si="6"/>
+        <v>2.032259064516129E-4</v>
+      </c>
+      <c r="D12" s="21">
+        <f t="shared" si="7"/>
+        <v>4920.6324993713097</v>
+      </c>
+      <c r="E12" s="21">
+        <f>$E$9*A12</f>
+        <v>0.39356099999999999</v>
+      </c>
+      <c r="F12" s="18">
+        <f t="shared" si="8"/>
+        <v>1.4246719914899715E-7</v>
+      </c>
+      <c r="G12" s="18">
+        <f>F12*SQRT(1+$H$5*B12/($H$4^2))</f>
+        <v>1.4246720552804948E-7</v>
+      </c>
+      <c r="H12" s="23">
+        <f t="shared" si="0"/>
+        <v>8.2010541656188505E-8</v>
+      </c>
+      <c r="I12" s="18">
+        <f t="shared" si="9"/>
+        <v>13.961678254208001</v>
+      </c>
+      <c r="J12" s="21">
+        <f>J$9*$C$9/$C12</f>
+        <v>39.682520156220242</v>
+      </c>
+      <c r="K12" s="28">
+        <f t="shared" si="1"/>
+        <v>0.77963087389949415</v>
+      </c>
+      <c r="L12" s="21">
+        <f>L$9*$C$9/$C12</f>
+        <v>198.41260078110119</v>
+      </c>
+      <c r="M12" s="28">
+        <f t="shared" si="2"/>
+        <v>0.34511113684944522</v>
+      </c>
+      <c r="N12" s="21">
+        <f>N$9*$C$9/$C12</f>
+        <v>992.06300390550598</v>
+      </c>
+      <c r="O12" s="28">
+        <f t="shared" si="3"/>
+        <v>0.15402661714854635</v>
+      </c>
+      <c r="P12" s="21">
+        <f>P$9*$C$9/$C12</f>
+        <v>19841.260078110121</v>
+      </c>
+      <c r="Q12" s="28">
+        <f t="shared" si="4"/>
+        <v>3.4424903297775374E-2</v>
+      </c>
+      <c r="R12" s="21">
+        <f t="shared" si="10"/>
+        <v>1000</v>
+      </c>
+      <c r="S12" s="28">
+        <f t="shared" si="4"/>
+        <v>0.15341353079087044</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="13">
+        <f t="shared" si="5"/>
+        <v>1.5811388300841896E-6</v>
+      </c>
+      <c r="B13" s="26">
+        <f t="shared" si="11"/>
+        <v>3.1622776601683795E-10</v>
+      </c>
+      <c r="C13" s="18">
+        <f t="shared" si="6"/>
+        <v>2.032261226793789E-4</v>
+      </c>
+      <c r="D13" s="21">
+        <f t="shared" si="7"/>
+        <v>4920.6272639352419</v>
+      </c>
+      <c r="E13" s="21">
+        <f>$E$9*A13</f>
+        <v>1.2445491582135275</v>
+      </c>
+      <c r="F13" s="18">
+        <f t="shared" si="8"/>
+        <v>8.0115193565604436E-8</v>
+      </c>
+      <c r="G13" s="18">
+        <f>F13*SQRT(1+$H$5*B13/($H$4^2))</f>
+        <v>8.0115204909341285E-8</v>
+      </c>
+      <c r="H13" s="23">
+        <f t="shared" si="0"/>
+        <v>2.5933982784596452E-7</v>
+      </c>
+      <c r="I13" s="18">
+        <f t="shared" si="9"/>
+        <v>4.4150660147414174</v>
+      </c>
+      <c r="J13" s="21">
+        <f>J$9*$C$9/$C13</f>
+        <v>39.682477934961625</v>
+      </c>
+      <c r="K13" s="28">
+        <f t="shared" si="1"/>
+        <v>0.61311681603932622</v>
+      </c>
+      <c r="L13" s="21">
+        <f>L$9*$C$9/$C13</f>
+        <v>198.41238967480814</v>
+      </c>
+      <c r="M13" s="28">
+        <f t="shared" si="2"/>
+        <v>0.27140207776372122</v>
+      </c>
+      <c r="N13" s="21">
+        <f>N$9*$C$9/$C13</f>
+        <v>992.06194837404064</v>
+      </c>
+      <c r="O13" s="28">
+        <f t="shared" si="3"/>
+        <v>0.12112951270262047</v>
+      </c>
+      <c r="P13" s="21">
+        <f>P$9*$C$9/$C13</f>
+        <v>19841.238967480815</v>
+      </c>
+      <c r="Q13" s="28">
+        <f t="shared" si="4"/>
+        <v>2.7072410187041481E-2</v>
+      </c>
+      <c r="R13" s="21">
+        <f t="shared" si="10"/>
+        <v>1000</v>
+      </c>
+      <c r="S13" s="28">
+        <f t="shared" si="4"/>
+        <v>0.12064730547773998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" s="13">
+        <f t="shared" si="5"/>
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="B14" s="26">
+        <f t="shared" si="11"/>
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="C14" s="18">
+        <f t="shared" si="6"/>
+        <v>2.0322680645161288E-4</v>
+      </c>
+      <c r="D14" s="21">
+        <f t="shared" si="7"/>
+        <v>4920.61070810604</v>
+      </c>
+      <c r="E14" s="21">
+        <f>$E$9*A14</f>
+        <v>3.9356100000000005</v>
+      </c>
+      <c r="F14" s="18">
+        <f t="shared" si="8"/>
+        <v>4.5052084117563321E-8</v>
+      </c>
+      <c r="G14" s="18">
+        <f>F14*SQRT(1+$H$5*B14/($H$4^2))</f>
+        <v>4.5052104289893915E-8</v>
+      </c>
+      <c r="H14" s="23">
+        <f t="shared" si="0"/>
+        <v>8.2010178468433995E-7</v>
+      </c>
+      <c r="I14" s="18">
+        <f t="shared" si="9"/>
+        <v>1.3961611438718891</v>
+      </c>
+      <c r="J14" s="21">
+        <f>J$9*$C$9/$C14</f>
+        <v>39.682344420210001</v>
+      </c>
+      <c r="K14" s="28">
+        <f>1/SQRT(J14-1)*SQRT(2*(1+2*SQRT(1+2*$I14)))</f>
+        <v>0.50306611627946463</v>
+      </c>
+      <c r="L14" s="21">
+        <f>L$9*$C$9/$C14</f>
+        <v>198.41172210105</v>
+      </c>
+      <c r="M14" s="28">
+        <f t="shared" si="2"/>
+        <v>0.22268706527812615</v>
+      </c>
+      <c r="N14" s="21">
+        <f>N$9*$C$9/$C14</f>
+        <v>992.05861050524993</v>
+      </c>
+      <c r="O14" s="28">
+        <f t="shared" si="3"/>
+        <v>9.9387505580269778E-2</v>
+      </c>
+      <c r="P14" s="21">
+        <f>P$9*$C$9/$C14</f>
+        <v>19841.172210105</v>
+      </c>
+      <c r="Q14" s="28">
+        <f t="shared" si="4"/>
+        <v>2.2213078003562148E-2</v>
+      </c>
+      <c r="R14" s="21">
+        <f t="shared" si="10"/>
+        <v>1000</v>
+      </c>
+      <c r="S14" s="28">
+        <f t="shared" si="4"/>
+        <v>9.8991684903721761E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" s="13">
+        <f t="shared" si="5"/>
+        <v>1.5811388300841898E-5</v>
+      </c>
+      <c r="B15" s="26">
+        <f t="shared" si="11"/>
+        <v>3.1622776601683795E-9</v>
+      </c>
+      <c r="C15" s="18">
+        <f t="shared" si="6"/>
+        <v>2.0322896872927305E-4</v>
+      </c>
+      <c r="D15" s="21">
+        <f t="shared" si="7"/>
+        <v>4920.5583547103843</v>
+      </c>
+      <c r="E15" s="21">
+        <f>$E$9*A15</f>
+        <v>12.445491582135276</v>
+      </c>
+      <c r="F15" s="18">
+        <f t="shared" si="8"/>
+        <v>2.533464868525764E-8</v>
+      </c>
+      <c r="G15" s="18">
+        <f>F15*SQRT(1+$H$5*B15/($H$4^2))</f>
+        <v>2.5334684557280423E-8</v>
+      </c>
+      <c r="H15" s="23">
+        <f t="shared" si="0"/>
+        <v>2.5933619601092542E-6</v>
+      </c>
+      <c r="I15" s="18">
+        <f t="shared" si="9"/>
+        <v>0.44149640892993097</v>
+      </c>
+      <c r="J15" s="21">
+        <f>J$9*$C$9/$C15</f>
+        <v>39.681922215406324</v>
+      </c>
+      <c r="K15" s="28">
+        <f t="shared" si="1"/>
+        <v>0.44000197639860561</v>
+      </c>
+      <c r="L15" s="21">
+        <f>L$9*$C$9/$C15</f>
+        <v>198.40961107703163</v>
+      </c>
+      <c r="M15" s="28">
+        <f t="shared" si="2"/>
+        <v>0.19477109436551371</v>
+      </c>
+      <c r="N15" s="21">
+        <f>N$9*$C$9/$C15</f>
+        <v>992.04805538515814</v>
+      </c>
+      <c r="O15" s="28">
+        <f t="shared" si="3"/>
+        <v>8.6928321526915681E-2</v>
+      </c>
+      <c r="P15" s="21">
+        <f>P$9*$C$9/$C15</f>
+        <v>19840.961107703162</v>
+      </c>
+      <c r="Q15" s="28">
+        <f t="shared" si="4"/>
+        <v>1.9428453965869005E-2</v>
+      </c>
+      <c r="R15" s="21">
+        <f t="shared" si="10"/>
+        <v>1000</v>
+      </c>
+      <c r="S15" s="28">
+        <f t="shared" si="4"/>
+        <v>8.658165973025049E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" s="13">
+        <f t="shared" si="5"/>
+        <v>5.0000000000000009E-5</v>
+      </c>
+      <c r="B16" s="26">
+        <f t="shared" si="11"/>
+        <v>1.0000000000000002E-8</v>
+      </c>
+      <c r="C16" s="18">
+        <f t="shared" si="6"/>
+        <v>2.0323580645161289E-4</v>
+      </c>
+      <c r="D16" s="21">
+        <f t="shared" si="7"/>
+        <v>4920.3928060682729</v>
+      </c>
+      <c r="E16" s="21">
+        <f>$E$9*A16</f>
+        <v>39.356100000000005</v>
+      </c>
+      <c r="F16" s="18">
+        <f t="shared" si="8"/>
+        <v>1.4246719914899715E-8</v>
+      </c>
+      <c r="G16" s="18">
+        <f>F16*SQRT(1+$H$5*B16/($H$4^2))</f>
+        <v>1.4246783705281577E-8</v>
+      </c>
+      <c r="H16" s="23">
+        <f t="shared" si="0"/>
+        <v>8.2006546767804566E-6</v>
+      </c>
+      <c r="I16" s="18">
+        <f t="shared" si="9"/>
+        <v>0.13959481959711473</v>
+      </c>
+      <c r="J16" s="21">
+        <f>J$9*$C$9/$C16</f>
+        <v>39.680587145711883</v>
+      </c>
+      <c r="K16" s="28">
+        <f t="shared" si="1"/>
+        <v>0.4106881131610875</v>
+      </c>
+      <c r="L16" s="21">
+        <f>L$9*$C$9/$C16</f>
+        <v>198.40293572855938</v>
+      </c>
+      <c r="M16" s="28">
+        <f t="shared" si="2"/>
+        <v>0.18179496812024343</v>
+      </c>
+      <c r="N16" s="21">
+        <f>N$9*$C$9/$C16</f>
+        <v>992.01467864279698</v>
+      </c>
+      <c r="O16" s="28">
+        <f t="shared" si="3"/>
+        <v>8.1136938793538033E-2</v>
+      </c>
+      <c r="P16" s="21">
+        <f>P$9*$C$9/$C16</f>
+        <v>19840.293572855939</v>
+      </c>
+      <c r="Q16" s="28">
+        <f t="shared" si="4"/>
+        <v>1.8134081357731698E-2</v>
+      </c>
+      <c r="R16" s="21">
+        <f t="shared" si="10"/>
+        <v>1000</v>
+      </c>
+      <c r="S16" s="28">
+        <f t="shared" si="4"/>
+        <v>8.081201163789406E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" s="13">
+        <f t="shared" si="5"/>
+        <v>1.58113883008419E-4</v>
+      </c>
+      <c r="B17" s="26">
+        <f t="shared" si="11"/>
+        <v>3.1622776601683799E-8</v>
+      </c>
+      <c r="C17" s="18">
+        <f t="shared" si="6"/>
+        <v>2.0325742922821459E-4</v>
+      </c>
+      <c r="D17" s="21">
+        <f t="shared" si="7"/>
+        <v>4919.8693685986455</v>
+      </c>
+      <c r="E17" s="21">
+        <f>$E$9*A17</f>
+        <v>124.45491582135278</v>
+      </c>
+      <c r="F17" s="18">
+        <f t="shared" si="8"/>
+        <v>8.0115193565604429E-9</v>
+      </c>
+      <c r="G17" s="18">
+        <f>F17*SQRT(1+$H$5*B17/($H$4^2))</f>
+        <v>8.0116327931339439E-9</v>
+      </c>
+      <c r="H17" s="23">
+        <f t="shared" si="0"/>
+        <v>2.592998832544368E-5</v>
+      </c>
+      <c r="I17" s="18">
+        <f t="shared" si="9"/>
+        <v>4.4093242679484043E-2</v>
+      </c>
+      <c r="J17" s="21">
+        <f>J$9*$C$9/$C17</f>
+        <v>39.676365875795526</v>
+      </c>
+      <c r="K17" s="28">
+        <f t="shared" si="1"/>
+        <v>0.39949642196259838</v>
+      </c>
+      <c r="L17" s="21">
+        <f>L$9*$C$9/$C17</f>
+        <v>198.38182937897764</v>
+      </c>
+      <c r="M17" s="28">
+        <f t="shared" si="2"/>
+        <v>0.17684066486890826</v>
+      </c>
+      <c r="N17" s="21">
+        <f>N$9*$C$9/$C17</f>
+        <v>991.90914689488818</v>
+      </c>
+      <c r="O17" s="28">
+        <f t="shared" si="3"/>
+        <v>7.8925765952944232E-2</v>
+      </c>
+      <c r="P17" s="21">
+        <f>P$9*$C$9/$C17</f>
+        <v>19838.182937897764</v>
+      </c>
+      <c r="Q17" s="28">
+        <f t="shared" si="4"/>
+        <v>1.7639883994937731E-2</v>
+      </c>
+      <c r="R17" s="21">
+        <f t="shared" si="10"/>
+        <v>1000</v>
+      </c>
+      <c r="S17" s="28">
+        <f t="shared" si="4"/>
+        <v>7.8605508199371232E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="13">
+        <f t="shared" si="5"/>
+        <v>5.0000000000000012E-4</v>
+      </c>
+      <c r="B18" s="26">
+        <f t="shared" si="11"/>
+        <v>1.0000000000000002E-7</v>
+      </c>
+      <c r="C18" s="18">
+        <f t="shared" si="6"/>
+        <v>2.033258064516129E-4</v>
+      </c>
+      <c r="D18" s="21">
+        <f t="shared" si="7"/>
+        <v>4918.2148466627532</v>
+      </c>
+      <c r="E18" s="21">
+        <f>$E$9*A18</f>
+        <v>393.56100000000009</v>
+      </c>
+      <c r="F18" s="18">
+        <f t="shared" si="8"/>
+        <v>4.5052084117563317E-9</v>
+      </c>
+      <c r="G18" s="18">
+        <f>F18*SQRT(1+$H$5*B18/($H$4^2))</f>
+        <v>4.5054101305915045E-9</v>
+      </c>
+      <c r="H18" s="23">
+        <f t="shared" si="0"/>
+        <v>8.1970247444379239E-5</v>
+      </c>
+      <c r="I18" s="18">
+        <f t="shared" si="9"/>
+        <v>1.3792126557194351E-2</v>
+      </c>
+      <c r="J18" s="21">
+        <f>J$9*$C$9/$C18</f>
+        <v>39.66302295695769</v>
+      </c>
+      <c r="K18" s="28">
+        <f t="shared" si="1"/>
+        <v>0.39573253243632511</v>
+      </c>
+      <c r="L18" s="21">
+        <f>L$9*$C$9/$C18</f>
+        <v>198.31511478478845</v>
+      </c>
+      <c r="M18" s="28">
+        <f>1/SQRT(L18-1)*SQRT(2*(1+2*SQRT(1+2*$I18)))</f>
+        <v>0.17517393294319702</v>
+      </c>
+      <c r="N18" s="21">
+        <f>N$9*$C$9/$C18</f>
+        <v>991.57557392394222</v>
+      </c>
+      <c r="O18" s="28">
+        <f t="shared" si="3"/>
+        <v>7.818183339066416E-2</v>
+      </c>
+      <c r="P18" s="21">
+        <f>P$9*$C$9/$C18</f>
+        <v>19831.511478478846</v>
+      </c>
+      <c r="Q18" s="28">
+        <f t="shared" si="4"/>
+        <v>1.7473612482116031E-2</v>
+      </c>
+      <c r="R18" s="21">
+        <f t="shared" si="10"/>
+        <v>1000</v>
+      </c>
+      <c r="S18" s="28">
+        <f t="shared" si="4"/>
+        <v>7.785148728954551E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="13">
+        <f t="shared" si="5"/>
+        <v>1.5811388300841901E-3</v>
+      </c>
+      <c r="B19" s="26">
+        <f t="shared" si="11"/>
+        <v>3.1622776601683802E-7</v>
+      </c>
+      <c r="C19" s="18">
+        <f t="shared" si="6"/>
+        <v>2.0354203421762973E-4</v>
+      </c>
+      <c r="D19" s="21">
+        <f t="shared" si="7"/>
+        <v>4912.990104691532</v>
+      </c>
+      <c r="E19" s="21">
+        <f>$E$9*A19</f>
+        <v>1244.549158213528</v>
+      </c>
+      <c r="F19" s="18">
+        <f t="shared" si="8"/>
+        <v>2.5334648685257636E-9</v>
+      </c>
+      <c r="G19" s="18">
+        <f>F19*SQRT(1+$H$5*B19/($H$4^2))</f>
+        <v>2.5338235636150378E-9</v>
+      </c>
+      <c r="H19" s="23">
+        <f t="shared" si="0"/>
+        <v>2.5893731421157233E-4</v>
+      </c>
+      <c r="I19" s="18">
+        <f t="shared" si="9"/>
+        <v>3.8915865059098095E-3</v>
+      </c>
+      <c r="J19" s="21">
+        <f>J$9*$C$9/$C19</f>
+        <v>39.620887941060737</v>
+      </c>
+      <c r="K19" s="28">
+        <f t="shared" si="1"/>
+        <v>0.39466266495356672</v>
+      </c>
+      <c r="L19" s="21">
+        <f>L$9*$C$9/$C19</f>
+        <v>198.10443970530369</v>
+      </c>
+      <c r="M19" s="28">
+        <f t="shared" si="2"/>
+        <v>0.1746984163210136</v>
+      </c>
+      <c r="N19" s="21">
+        <f>N$9*$C$9/$C19</f>
+        <v>990.52219852651842</v>
+      </c>
+      <c r="O19" s="28">
+        <f t="shared" si="3"/>
+        <v>7.7969437427295785E-2</v>
+      </c>
+      <c r="P19" s="21">
+        <f>P$9*$C$9/$C19</f>
+        <v>19810.44397053037</v>
+      </c>
+      <c r="Q19" s="28">
+        <f t="shared" si="4"/>
+        <v>1.7426133171558531E-2</v>
+      </c>
+      <c r="R19" s="21">
+        <f t="shared" si="10"/>
+        <v>1000</v>
+      </c>
+      <c r="S19" s="28">
+        <f t="shared" si="4"/>
+        <v>7.7598696716931398E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" s="13">
+        <f t="shared" si="5"/>
+        <v>5.0000000000000018E-3</v>
+      </c>
+      <c r="B20" s="26">
+        <f t="shared" si="11"/>
+        <v>1.0000000000000004E-6</v>
+      </c>
+      <c r="C20" s="18">
+        <f t="shared" si="6"/>
+        <v>2.0422580645161289E-4</v>
+      </c>
+      <c r="D20" s="21">
+        <f t="shared" si="7"/>
+        <v>4896.5408308324122</v>
+      </c>
+      <c r="E20" s="21">
+        <f>$E$9*A20</f>
+        <v>3935.6100000000015</v>
+      </c>
+      <c r="F20" s="18">
+        <f t="shared" si="8"/>
+        <v>1.4246719914899713E-9</v>
+      </c>
+      <c r="G20" s="18">
+        <f>F20*SQRT(1+$H$5*B20/($H$4^2))</f>
+        <v>1.425309753987723E-9</v>
+      </c>
+      <c r="H20" s="23">
+        <f t="shared" si="0"/>
+        <v>8.1609013847206899E-4</v>
+      </c>
+      <c r="I20" s="18">
+        <f t="shared" si="9"/>
+        <v>-2.4160410561884903E-4</v>
+      </c>
+      <c r="J20" s="21">
+        <f>J$9*$C$9/$C20</f>
+        <v>39.488232506713004</v>
+      </c>
+      <c r="K20" s="28">
+        <f t="shared" si="1"/>
+        <v>0.3947995587785344</v>
+      </c>
+      <c r="L20" s="21">
+        <f>L$9*$C$9/$C20</f>
+        <v>197.44116253356501</v>
+      </c>
+      <c r="M20" s="28">
+        <f t="shared" si="2"/>
+        <v>0.17475290122012424</v>
+      </c>
+      <c r="N20" s="21">
+        <f>N$9*$C$9/$C20</f>
+        <v>987.20581266782494</v>
+      </c>
+      <c r="O20" s="28">
+        <f t="shared" si="3"/>
+        <v>7.7993222258025879E-2</v>
+      </c>
+      <c r="P20" s="21">
+        <f>P$9*$C$9/$C20</f>
+        <v>19744.1162533565</v>
+      </c>
+      <c r="Q20" s="28">
+        <f t="shared" si="4"/>
+        <v>1.7431420958895105E-2</v>
+      </c>
+      <c r="R20" s="21">
+        <f t="shared" si="10"/>
+        <v>1000</v>
+      </c>
+      <c r="S20" s="28">
+        <f t="shared" si="4"/>
+        <v>7.7492183511045365E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="13">
+        <f t="shared" si="5"/>
+        <v>1.5811388300841903E-2</v>
+      </c>
+      <c r="B21" s="26">
+        <f t="shared" si="11"/>
+        <v>3.1622776601683809E-6</v>
+      </c>
+      <c r="C21" s="18">
+        <f t="shared" si="6"/>
+        <v>2.0638808411178126E-4</v>
+      </c>
+      <c r="D21" s="21">
+        <f t="shared" si="7"/>
+        <v>4845.2409658417728</v>
+      </c>
+      <c r="E21" s="21">
+        <f>$E$9*A21</f>
+        <v>12445.491582135281</v>
+      </c>
+      <c r="F21" s="18">
+        <f t="shared" si="8"/>
+        <v>8.0115193565604408E-10</v>
+      </c>
+      <c r="G21" s="18">
+        <f>F21*SQRT(1+$H$5*B21/($H$4^2))</f>
+        <v>8.0228550746100921E-10</v>
+      </c>
+      <c r="H21" s="23">
+        <f t="shared" si="0"/>
+        <v>2.5536662107356841E-3</v>
+      </c>
+      <c r="I21" s="18">
+        <f t="shared" si="9"/>
+        <v>-4.6713588501707008E-3</v>
+      </c>
+      <c r="J21" s="21">
+        <f>J$9*$C$9/$C21</f>
+        <v>39.07452391807881</v>
+      </c>
+      <c r="K21" s="28">
+        <f t="shared" si="1"/>
+        <v>0.39635057158629527</v>
+      </c>
+      <c r="L21" s="21">
+        <f>L$9*$C$9/$C21</f>
+        <v>195.37261959039404</v>
+      </c>
+      <c r="M21" s="28">
+        <f t="shared" si="2"/>
+        <v>0.1754200319527382</v>
+      </c>
+      <c r="N21" s="21">
+        <f>N$9*$C$9/$C21</f>
+        <v>976.86309795197019</v>
+      </c>
+      <c r="O21" s="28">
+        <f t="shared" si="3"/>
+        <v>7.8289276909153743E-2</v>
+      </c>
+      <c r="P21" s="21">
+        <f>P$9*$C$9/$C21</f>
+        <v>19537.261959039406</v>
+      </c>
+      <c r="Q21" s="28">
+        <f t="shared" si="4"/>
+        <v>1.7497499696060136E-2</v>
+      </c>
+      <c r="R21" s="21">
+        <f t="shared" si="10"/>
+        <v>1000</v>
+      </c>
+      <c r="S21" s="28">
+        <f t="shared" si="4"/>
+        <v>7.7377373787919007E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" s="13">
+        <f t="shared" si="5"/>
+        <v>5.0000000000000031E-2</v>
+      </c>
+      <c r="B22" s="26">
+        <f t="shared" si="11"/>
+        <v>1.0000000000000006E-5</v>
+      </c>
+      <c r="C22" s="18">
+        <f t="shared" si="6"/>
+        <v>2.1322580645161289E-4</v>
+      </c>
+      <c r="D22" s="21">
+        <f t="shared" si="7"/>
+        <v>4689.863842662633</v>
+      </c>
+      <c r="E22" s="21">
+        <f>$E$9*A22</f>
+        <v>39356.100000000028</v>
+      </c>
+      <c r="F22" s="18">
+        <f t="shared" si="8"/>
+        <v>4.5052084117563311E-10</v>
+      </c>
+      <c r="G22" s="18">
+        <f>F22*SQRT(1+$H$5*B22/($H$4^2))</f>
+        <v>4.5253357865482525E-10</v>
+      </c>
+      <c r="H22" s="23">
+        <f t="shared" si="0"/>
+        <v>7.8164397377710575E-3</v>
+      </c>
+      <c r="I22" s="18">
+        <f t="shared" si="9"/>
+        <v>-1.5498618826354831E-2</v>
+      </c>
+      <c r="J22" s="21">
+        <f>J$9*$C$9/$C22</f>
+        <v>37.821482602118003</v>
+      </c>
+      <c r="K22" s="28">
+        <f t="shared" si="1"/>
+        <v>0.40156126746848231</v>
+      </c>
+      <c r="L22" s="21">
+        <f>L$9*$C$9/$C22</f>
+        <v>189.10741301059002</v>
+      </c>
+      <c r="M22" s="28">
+        <f t="shared" si="2"/>
+        <v>0.17766402488072741</v>
+      </c>
+      <c r="N22" s="21">
+        <f>N$9*$C$9/$C22</f>
+        <v>945.53706505295008</v>
+      </c>
+      <c r="O22" s="28">
+        <f t="shared" si="3"/>
+        <v>7.9285350324502346E-2</v>
+      </c>
+      <c r="P22" s="21">
+        <f>P$9*$C$9/$C22</f>
+        <v>18910.741301059003</v>
+      </c>
+      <c r="Q22" s="28">
+        <f t="shared" si="4"/>
+        <v>1.7719834373656904E-2</v>
+      </c>
+      <c r="R22" s="21">
+        <f t="shared" si="10"/>
+        <v>1000</v>
+      </c>
+      <c r="S22" s="28">
+        <f t="shared" si="4"/>
+        <v>7.709384526724021E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23" s="13">
+        <f t="shared" si="5"/>
+        <v>0.15811388300841908</v>
+      </c>
+      <c r="B23" s="26">
+        <f t="shared" si="11"/>
+        <v>3.1622776601683816E-5</v>
+      </c>
+      <c r="C23" s="18">
+        <f t="shared" si="6"/>
+        <v>2.3484858305329671E-4</v>
+      </c>
+      <c r="D23" s="21">
+        <f t="shared" si="7"/>
+        <v>4258.0627355671941</v>
+      </c>
+      <c r="E23" s="21">
+        <f>$E$9*A23</f>
+        <v>124454.91582135284</v>
+      </c>
+      <c r="F23" s="18">
+        <f t="shared" si="8"/>
+        <v>2.5334648685257626E-10</v>
+      </c>
+      <c r="G23" s="18">
+        <f>F23*SQRT(1+$H$5*B23/($H$4^2))</f>
+        <v>2.5690864889506054E-10</v>
+      </c>
+      <c r="H23" s="23">
+        <f t="shared" si="0"/>
+        <v>2.2441961107132674E-2</v>
+      </c>
+      <c r="I23" s="18">
+        <f t="shared" si="9"/>
+        <v>-4.484463453330087E-2</v>
+      </c>
+      <c r="J23" s="21">
+        <f>J$9*$C$9/$C23</f>
+        <v>34.339215609412854</v>
+      </c>
+      <c r="K23" s="28">
+        <f t="shared" si="1"/>
+        <v>0.41768583847114615</v>
+      </c>
+      <c r="L23" s="21">
+        <f>L$9*$C$9/$C23</f>
+        <v>171.69607804706428</v>
+      </c>
+      <c r="M23" s="28">
+        <f t="shared" si="2"/>
+        <v>0.18459318716231499</v>
+      </c>
+      <c r="N23" s="21">
+        <f>N$9*$C$9/$C23</f>
+        <v>858.48039023532135</v>
+      </c>
+      <c r="O23" s="28">
+        <f t="shared" si="3"/>
+        <v>8.2359810990037627E-2</v>
+      </c>
+      <c r="P23" s="21">
+        <f>P$9*$C$9/$C23</f>
+        <v>17169.607804706429</v>
+      </c>
+      <c r="Q23" s="28">
+        <f t="shared" si="4"/>
+        <v>1.8406020433312568E-2</v>
+      </c>
+      <c r="R23" s="21">
+        <f t="shared" si="10"/>
+        <v>1000</v>
+      </c>
+      <c r="S23" s="28">
+        <f t="shared" si="4"/>
+        <v>7.6303541527017807E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24" s="13">
+        <f t="shared" si="5"/>
+        <v>0.50000000000000033</v>
+      </c>
+      <c r="B24" s="26">
+        <f t="shared" si="11"/>
+        <v>1.0000000000000007E-4</v>
+      </c>
+      <c r="C24" s="18">
+        <f t="shared" si="6"/>
+        <v>3.0322580645161297E-4</v>
+      </c>
+      <c r="D24" s="21">
+        <f t="shared" si="7"/>
+        <v>3297.8723404255311</v>
+      </c>
+      <c r="E24" s="21">
+        <f>$E$9*A24</f>
+        <v>393561.00000000029</v>
+      </c>
+      <c r="F24" s="18">
+        <f t="shared" si="8"/>
+        <v>1.4246719914899709E-10</v>
+      </c>
+      <c r="G24" s="18">
+        <f>F24*SQRT(1+$H$5*B24/($H$4^2))</f>
+        <v>1.487094963675921E-10</v>
+      </c>
+      <c r="H24" s="23">
+        <f t="shared" si="0"/>
+        <v>5.4964539007092222E-2</v>
+      </c>
+      <c r="I24" s="18">
+        <f t="shared" si="9"/>
+        <v>-0.10991888275820841</v>
+      </c>
+      <c r="J24" s="21">
+        <f>J$9*$C$9/$C24</f>
+        <v>26.595744680851059</v>
+      </c>
+      <c r="K24" s="28">
+        <f t="shared" si="1"/>
+        <v>0.46494251976350837</v>
+      </c>
+      <c r="L24" s="21">
+        <f>L$9*$C$9/$C24</f>
+        <v>132.97872340425528</v>
+      </c>
+      <c r="M24" s="28">
+        <f t="shared" si="2"/>
+        <v>0.20475343108641028</v>
+      </c>
+      <c r="N24" s="21">
+        <f>N$9*$C$9/$C24</f>
+        <v>664.89361702127644</v>
+      </c>
+      <c r="O24" s="28">
+        <f t="shared" si="3"/>
+        <v>9.1292248357472849E-2</v>
+      </c>
+      <c r="P24" s="21">
+        <f>P$9*$C$9/$C24</f>
+        <v>13297.872340425529</v>
+      </c>
+      <c r="Q24" s="28">
+        <f t="shared" si="4"/>
+        <v>2.0398977551644208E-2</v>
+      </c>
+      <c r="R24" s="21">
+        <f t="shared" si="10"/>
+        <v>1000</v>
+      </c>
+      <c r="S24" s="28">
+        <f t="shared" si="4"/>
+        <v>7.4421840386514823E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A25" s="13">
+        <f t="shared" si="5"/>
+        <v>1.5811388300841906</v>
+      </c>
+      <c r="B25" s="26">
+        <f t="shared" si="11"/>
+        <v>3.1622776601683816E-4</v>
+      </c>
+      <c r="C25" s="18">
+        <f t="shared" si="6"/>
+        <v>5.1945357246845102E-4</v>
+      </c>
+      <c r="D25" s="21">
+        <f t="shared" si="7"/>
+        <v>1925.0998607016702</v>
+      </c>
+      <c r="E25" s="21">
+        <f>$E$9*A25</f>
+        <v>1244549.1582135283</v>
+      </c>
+      <c r="F25" s="18">
+        <f t="shared" si="8"/>
+        <v>8.0115193565604403E-11</v>
+      </c>
+      <c r="G25" s="18">
+        <f>F25*SQRT(1+$H$5*B25/($H$4^2))</f>
+        <v>9.075271740613142E-11</v>
+      </c>
+      <c r="H25" s="23">
+        <f t="shared" si="0"/>
+        <v>0.10146167138483592</v>
+      </c>
+      <c r="I25" s="18">
+        <f t="shared" si="9"/>
+        <v>-0.20292112631207646</v>
+      </c>
+      <c r="J25" s="21">
+        <f>J$9*$C$9/$C25</f>
+        <v>15.524998876626372</v>
+      </c>
+      <c r="K25" s="28">
+        <f t="shared" si="1"/>
+        <v>0.59157978868824668</v>
+      </c>
+      <c r="L25" s="21">
+        <f>L$9*$C$9/$C25</f>
+        <v>77.624994383131863</v>
+      </c>
+      <c r="M25" s="28">
+        <f t="shared" si="2"/>
+        <v>0.25756458872783095</v>
+      </c>
+      <c r="N25" s="21">
+        <f>N$9*$C$9/$C25</f>
+        <v>388.12497191565927</v>
+      </c>
+      <c r="O25" s="28">
+        <f t="shared" si="3"/>
+        <v>0.11458975429943791</v>
+      </c>
+      <c r="P25" s="21">
+        <f>P$9*$C$9/$C25</f>
+        <v>7762.4994383131861</v>
+      </c>
+      <c r="Q25" s="28">
+        <f t="shared" si="4"/>
+        <v>2.5591666434572197E-2</v>
+      </c>
+      <c r="R25" s="21">
+        <f t="shared" si="10"/>
+        <v>1000</v>
+      </c>
+      <c r="S25" s="28">
+        <f t="shared" si="4"/>
+        <v>7.1332695863044776E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A26" s="13">
+        <f t="shared" si="5"/>
+        <v>5.0000000000000036</v>
+      </c>
+      <c r="B26" s="26">
+        <f t="shared" si="11"/>
+        <v>1.0000000000000007E-3</v>
+      </c>
+      <c r="C26" s="18">
+        <f t="shared" si="6"/>
+        <v>1.2032258064516136E-3</v>
+      </c>
+      <c r="D26" s="21">
+        <f t="shared" si="7"/>
+        <v>831.09919571045521</v>
+      </c>
+      <c r="E26" s="21">
+        <f t="shared" ref="E26:E30" si="12">$E$9*A26</f>
+        <v>3935610.0000000028</v>
+      </c>
+      <c r="F26" s="18">
+        <f t="shared" si="8"/>
+        <v>4.5052084117563306E-11</v>
+      </c>
+      <c r="G26" s="18">
+        <f t="shared" ref="G26:G30" si="13">F26*SQRT(1+$H$5*B26/($H$4^2))</f>
+        <v>6.2026621380491823E-11</v>
+      </c>
+      <c r="H26" s="23">
+        <f t="shared" ref="H26:H30" si="14">1/6*B26/C26</f>
+        <v>0.13851653261840929</v>
+      </c>
+      <c r="I26" s="18">
+        <f t="shared" ref="I26:I30" si="15">G26^2/($H$5*C26)-2*H26</f>
+        <v>-0.27703261824867703</v>
+      </c>
+      <c r="J26" s="21">
+        <f t="shared" ref="J26:J30" si="16">J$9*$C$9/$C26</f>
+        <v>6.7024128686327034</v>
+      </c>
+      <c r="K26" s="28">
+        <f t="shared" si="1"/>
+        <v>0.90506928878312853</v>
+      </c>
+      <c r="L26" s="21">
+        <f t="shared" ref="L26:L30" si="17">L$9*$C$9/$C26</f>
+        <v>33.512064343163516</v>
+      </c>
+      <c r="M26" s="28">
+        <f t="shared" si="2"/>
+        <v>0.37904335255605892</v>
+      </c>
+      <c r="N26" s="21">
+        <f t="shared" ref="N26:N30" si="18">N$9*$C$9/$C26</f>
+        <v>167.56032171581759</v>
+      </c>
+      <c r="O26" s="28">
+        <f t="shared" si="3"/>
+        <v>0.16746551216463765</v>
+      </c>
+      <c r="P26" s="21">
+        <f t="shared" ref="P26:R30" si="19">P$9*$C$9/$C26</f>
+        <v>3351.206434316352</v>
+      </c>
+      <c r="Q26" s="28">
+        <f t="shared" si="4"/>
+        <v>3.7340091112431854E-2</v>
+      </c>
+      <c r="R26" s="21">
+        <f t="shared" si="10"/>
+        <v>1000</v>
+      </c>
+      <c r="S26" s="28">
+        <f t="shared" si="4"/>
+        <v>6.8379892452244295E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A27" s="13">
+        <f t="shared" si="5"/>
+        <v>15.811388300841907</v>
+      </c>
+      <c r="B27" s="26">
+        <f t="shared" si="11"/>
+        <v>3.1622776601683816E-3</v>
+      </c>
+      <c r="C27" s="18">
+        <f t="shared" si="6"/>
+        <v>3.3655034666199945E-3</v>
+      </c>
+      <c r="D27" s="21">
+        <f t="shared" si="7"/>
+        <v>297.13236367701887</v>
+      </c>
+      <c r="E27" s="21">
+        <f t="shared" si="12"/>
+        <v>12445491.582135284</v>
+      </c>
+      <c r="F27" s="18">
+        <f t="shared" si="8"/>
+        <v>2.5334648685257628E-11</v>
+      </c>
+      <c r="G27" s="18">
+        <f t="shared" si="13"/>
+        <v>4.9592901715349459E-11</v>
+      </c>
+      <c r="H27" s="23">
+        <f t="shared" si="14"/>
+        <v>0.15660250596147732</v>
+      </c>
+      <c r="I27" s="18">
+        <f t="shared" si="15"/>
+        <v>-0.3132049097641304</v>
+      </c>
+      <c r="J27" s="21">
+        <f t="shared" si="16"/>
+        <v>2.3962287393307973</v>
+      </c>
+      <c r="K27" s="28">
+        <f t="shared" si="1"/>
+        <v>1.7842338748626434</v>
+      </c>
+      <c r="L27" s="21">
+        <f t="shared" si="17"/>
+        <v>11.981143696653987</v>
+      </c>
+      <c r="M27" s="28">
+        <f t="shared" si="2"/>
+        <v>0.63621847992419422</v>
+      </c>
+      <c r="N27" s="21">
+        <f t="shared" si="18"/>
+        <v>59.905718483269929</v>
+      </c>
+      <c r="O27" s="28">
+        <f t="shared" si="3"/>
+        <v>0.27469536925678029</v>
+      </c>
+      <c r="P27" s="21">
+        <f t="shared" si="19"/>
+        <v>1198.1143696653987</v>
+      </c>
+      <c r="Q27" s="28">
+        <f t="shared" si="4"/>
+        <v>6.0934358738225301E-2</v>
+      </c>
+      <c r="R27" s="21">
+        <f t="shared" si="10"/>
+        <v>1000</v>
+      </c>
+      <c r="S27" s="28">
+        <f t="shared" si="4"/>
+        <v>6.670330041299799E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A28" s="13">
+        <f t="shared" si="5"/>
+        <v>50.000000000000036</v>
+      </c>
+      <c r="B28" s="26">
+        <f t="shared" si="11"/>
+        <v>1.0000000000000007E-2</v>
+      </c>
+      <c r="C28" s="18">
+        <f t="shared" si="6"/>
+        <v>1.0203225806451621E-2</v>
+      </c>
+      <c r="D28" s="21">
+        <f t="shared" si="7"/>
+        <v>98.008220044261705</v>
+      </c>
+      <c r="E28" s="21">
+        <f t="shared" si="12"/>
+        <v>39356100.00000003</v>
+      </c>
+      <c r="F28" s="18">
+        <f t="shared" si="8"/>
+        <v>1.424671991489971E-11</v>
+      </c>
+      <c r="G28" s="18">
+        <f t="shared" si="13"/>
+        <v>4.4950867676569777E-11</v>
+      </c>
+      <c r="H28" s="23">
+        <f t="shared" si="14"/>
+        <v>0.16334703340710297</v>
+      </c>
+      <c r="I28" s="18">
+        <f t="shared" si="15"/>
+        <v>-0.32669403913041578</v>
+      </c>
+      <c r="J28" s="21">
+        <f t="shared" si="16"/>
+        <v>0.79038887132469116</v>
+      </c>
+      <c r="K28" s="28" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="L28" s="21">
+        <f t="shared" si="17"/>
+        <v>3.9519443566234558</v>
+      </c>
+      <c r="M28" s="28">
+        <f t="shared" si="2"/>
+        <v>1.2146118568344582</v>
+      </c>
+      <c r="N28" s="21">
+        <f t="shared" si="18"/>
+        <v>19.759721783117278</v>
+      </c>
+      <c r="O28" s="28">
+        <f t="shared" si="3"/>
+        <v>0.48181287732623052</v>
+      </c>
+      <c r="P28" s="21">
+        <f t="shared" si="19"/>
+        <v>395.1944356623456</v>
+      </c>
+      <c r="Q28" s="28">
+        <f t="shared" si="4"/>
+        <v>0.1051081409931628</v>
+      </c>
+      <c r="R28" s="21">
+        <f t="shared" si="10"/>
+        <v>1000</v>
+      </c>
+      <c r="S28" s="28">
+        <f t="shared" si="4"/>
+        <v>6.6025067769599086E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A29" s="13">
+        <f t="shared" si="5"/>
+        <v>158.11388300841909</v>
+      </c>
+      <c r="B29" s="26">
+        <f t="shared" si="11"/>
+        <v>3.1622776601683819E-2</v>
+      </c>
+      <c r="C29" s="18">
+        <f t="shared" si="6"/>
+        <v>3.1826002408135434E-2</v>
+      </c>
+      <c r="D29" s="21">
+        <f t="shared" si="7"/>
+        <v>31.420848499162364</v>
+      </c>
+      <c r="E29" s="21">
+        <f t="shared" si="12"/>
+        <v>124454915.82135285</v>
+      </c>
+      <c r="F29" s="18">
+        <f t="shared" si="8"/>
+        <v>8.0115193565604403E-12</v>
+      </c>
+      <c r="G29" s="18">
+        <f t="shared" si="13"/>
+        <v>4.3379671724707973E-11</v>
+      </c>
+      <c r="H29" s="23">
+        <f t="shared" si="14"/>
+        <v>0.16560241212072727</v>
+      </c>
+      <c r="I29" s="18">
+        <f t="shared" si="15"/>
+        <v>-0.33120481597579865</v>
+      </c>
+      <c r="J29" s="21">
+        <f t="shared" si="16"/>
+        <v>0.25339393950937389</v>
+      </c>
+      <c r="K29" s="28" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="L29" s="21">
+        <f t="shared" si="17"/>
+        <v>1.2669696975468694</v>
+      </c>
+      <c r="M29" s="28">
+        <f t="shared" si="2"/>
+        <v>4.0245463608599676</v>
+      </c>
+      <c r="N29" s="21">
+        <f t="shared" si="18"/>
+        <v>6.3348484877343472</v>
+      </c>
+      <c r="O29" s="28">
+        <f t="shared" si="3"/>
+        <v>0.9002992212355333</v>
+      </c>
+      <c r="P29" s="21">
+        <f t="shared" si="19"/>
+        <v>126.69696975468695</v>
+      </c>
+      <c r="Q29" s="28">
+        <f t="shared" si="4"/>
+        <v>0.18547505790524033</v>
+      </c>
+      <c r="R29" s="21">
+        <f t="shared" si="10"/>
+        <v>1000</v>
+      </c>
+      <c r="S29" s="28">
+        <f t="shared" si="4"/>
+        <v>6.5790801197085372E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A30" s="13">
+        <f t="shared" si="5"/>
+        <v>500.0000000000004</v>
+      </c>
+      <c r="B30" s="26">
+        <f t="shared" si="11"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="C30" s="18">
+        <f t="shared" si="6"/>
+        <v>0.1002032258064517</v>
+      </c>
+      <c r="D30" s="21">
+        <f t="shared" si="7"/>
+        <v>9.9797186363197277</v>
+      </c>
+      <c r="E30" s="21">
+        <f t="shared" si="12"/>
+        <v>393561000.0000003</v>
+      </c>
+      <c r="F30" s="18">
+        <f t="shared" si="8"/>
+        <v>4.5052084117563309E-12</v>
+      </c>
+      <c r="G30" s="18">
+        <f t="shared" si="13"/>
+        <v>4.2870833667847492E-11</v>
+      </c>
+      <c r="H30" s="23">
+        <f t="shared" si="14"/>
+        <v>0.16632864393866229</v>
+      </c>
+      <c r="I30" s="18">
+        <f t="shared" si="15"/>
+        <v>-0.3326572853132595</v>
+      </c>
+      <c r="J30" s="21">
+        <f t="shared" si="16"/>
+        <v>8.0481601905804251E-2</v>
+      </c>
+      <c r="K30" s="28" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="L30" s="21">
+        <f t="shared" si="17"/>
+        <v>0.40240800952902128</v>
+      </c>
+      <c r="M30" s="28" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N30" s="21">
+        <f t="shared" si="18"/>
+        <v>2.0120400476451064</v>
+      </c>
+      <c r="O30" s="28">
+        <f t="shared" si="3"/>
+        <v>2.0646443628961766</v>
+      </c>
+      <c r="P30" s="21">
+        <f t="shared" si="19"/>
+        <v>40.240800952902127</v>
+      </c>
+      <c r="Q30" s="28">
+        <f t="shared" si="4"/>
+        <v>0.3315699565126673</v>
+      </c>
+      <c r="R30" s="21">
+        <f t="shared" si="10"/>
+        <v>1000</v>
+      </c>
+      <c r="S30" s="28">
+        <f t="shared" si="4"/>
+        <v>6.5714523001147801E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D31" s="22"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D32" s="22"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D33" s="22"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D34" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>